<commit_message>
Added cellobiose, urea, misc, and spring squirrel CRDS info + metadata
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\CRDS_Calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93503290-009B-440C-B0D7-B9E85C7F2702}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19248" windowHeight="9024" xr2:uid="{1703010F-427F-4A34-A709-A1B3C21EF1FA}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="98">
   <si>
     <t>Number</t>
   </si>
@@ -243,6 +244,81 @@
   </si>
   <si>
     <t>Antibiotics</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>P07</t>
+  </si>
+  <si>
+    <t>P08</t>
+  </si>
+  <si>
+    <t>P09</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>Urea</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>W01</t>
+  </si>
+  <si>
+    <t>W38</t>
+  </si>
+  <si>
+    <t>W39</t>
   </si>
 </sst>
 </file>
@@ -278,10 +354,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9715411-D9A2-427F-BF3E-80D304B834E6}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,30 +766,30 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4022</v>
+        <v>3995</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3991</v>
+        <v>4022</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -722,21 +801,21 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4016</v>
+        <v>3991</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -747,10 +826,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4029</v>
+        <v>4016</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>68</v>
@@ -762,15 +841,15 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3992</v>
+        <v>4029</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
@@ -779,38 +858,38 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>3967</v>
+        <v>3992</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" t="s">
         <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4031</v>
+        <v>4026</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>92</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
@@ -822,15 +901,15 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>4044</v>
+        <v>3967</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
@@ -839,27 +918,27 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3966</v>
+        <v>4031</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
         <v>70</v>
@@ -867,10 +946,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3983</v>
+        <v>4044</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
         <v>68</v>
@@ -879,7 +958,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
         <v>70</v>
@@ -887,10 +966,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>4045</v>
+        <v>3978</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
@@ -902,35 +981,35 @@
         <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>4002</v>
+        <v>3966</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>68</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
         <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>4043</v>
+        <v>3983</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
@@ -939,58 +1018,58 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>4030</v>
+        <v>4045</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>71</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>4037</v>
+        <v>4032</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
         <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>4000</v>
+        <v>4002</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
@@ -999,18 +1078,18 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>4010</v>
+        <v>4043</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
         <v>68</v>
@@ -1019,58 +1098,58 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>4038</v>
+        <v>4030</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>71</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>4036</v>
+        <v>4037</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
         <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>4007</v>
+        <v>4000</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
         <v>68</v>
@@ -1087,70 +1166,70 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>3973</v>
+        <v>4010</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
         <v>68</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
         <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>4008</v>
+        <v>4038</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>3982</v>
+        <v>4036</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>4019</v>
+        <v>4007</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>68</v>
@@ -1159,21 +1238,21 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>4013</v>
+      <c r="A29">
+        <v>3973</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -1182,75 +1261,75 @@
         <v>71</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>4056</v>
+        <v>4008</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>4005</v>
+        <v>3982</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
         <v>71</v>
       </c>
       <c r="F31" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>4040</v>
+        <v>4019</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
         <v>71</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>3986</v>
+        <v>4034</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1262,35 +1341,35 @@
         <v>71</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>3996</v>
+      <c r="A34" s="1">
+        <v>4013</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
         <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>4047</v>
+        <v>4056</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1302,15 +1381,15 @@
         <v>71</v>
       </c>
       <c r="F35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>3971</v>
+        <v>4005</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1327,10 +1406,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>4028</v>
+        <v>4040</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1347,10 +1426,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>4006</v>
+        <v>3986</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -1362,41 +1441,41 @@
         <v>71</v>
       </c>
       <c r="F38" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>4042</v>
+        <v>3996</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
         <v>71</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>3979</v>
+        <v>4047</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
         <v>71</v>
@@ -1407,36 +1486,36 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>4035</v>
+        <v>3971</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E41" t="s">
         <v>71</v>
       </c>
       <c r="F41" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>4048</v>
+        <v>4028</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E42" t="s">
         <v>71</v>
@@ -1447,10 +1526,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>3997</v>
+        <v>4006</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1459,27 +1538,27 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>4011</v>
+        <v>4042</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F44" t="s">
         <v>69</v>
@@ -1487,70 +1566,70 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>3970</v>
+        <v>3979</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3969</v>
+        <v>4035</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>4041</v>
+        <v>4048</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F47" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>3976</v>
+        <v>3997</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -1567,30 +1646,30 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>4039</v>
+        <v>4011</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>3974</v>
+        <v>3970</v>
       </c>
       <c r="B50" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1602,15 +1681,15 @@
         <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>4021</v>
+        <v>3969</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1627,10 +1706,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>3980</v>
+        <v>4041</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1647,10 +1726,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>4054</v>
+        <v>3976</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
@@ -1662,15 +1741,15 @@
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>3989</v>
+        <v>4039</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -1682,15 +1761,15 @@
         <v>8</v>
       </c>
       <c r="F54" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>4050</v>
+        <v>3974</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
@@ -1702,15 +1781,15 @@
         <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>3975</v>
+        <v>4021</v>
       </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -1722,15 +1801,15 @@
         <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>4014</v>
+        <v>3980</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
@@ -1742,15 +1821,15 @@
         <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>4017</v>
+        <v>4054</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
@@ -1762,26 +1841,486 @@
         <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
+        <v>3989</v>
+      </c>
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>4050</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>3975</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>4014</v>
+      </c>
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>4017</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>4004</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>67</v>
       </c>
-      <c r="C59" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" t="s">
-        <v>8</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>4003</v>
+      </c>
+      <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>4055</v>
+      </c>
+      <c r="B66" t="s">
+        <v>97</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>3998</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>3968</v>
+      </c>
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>3987</v>
+      </c>
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" t="s">
+        <v>89</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>3957</v>
+      </c>
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" t="s">
+        <v>89</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>4023</v>
+      </c>
+      <c r="B71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71" t="s">
+        <v>89</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" t="s">
+        <v>71</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>3993</v>
+      </c>
+      <c r="B72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" t="s">
+        <v>89</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E72" t="s">
+        <v>71</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>4033</v>
+      </c>
+      <c r="B73" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" t="s">
+        <v>89</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>3985</v>
+      </c>
+      <c r="B74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74" t="s">
+        <v>89</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>3999</v>
+      </c>
+      <c r="B75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>3984</v>
+      </c>
+      <c r="B76" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" t="s">
+        <v>8</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>3990</v>
+      </c>
+      <c r="B77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77" t="s">
+        <v>89</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>4012</v>
+      </c>
+      <c r="B78" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78" t="s">
+        <v>89</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>4015</v>
+      </c>
+      <c r="B79" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>4053</v>
+      </c>
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" t="s">
+        <v>89</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>4025</v>
+      </c>
+      <c r="B81" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81" t="s">
+        <v>89</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" t="s">
+        <v>8</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>4046</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" t="s">
+        <v>89</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2019 CRDS vals; separated urea from carb project
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\CRDS_Calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3B5CA-6914-4CF3-9021-66C04D80A698}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9FAF145-0EBC-457E-8282-494011A72767}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19248" windowHeight="9024" xr2:uid="{1703010F-427F-4A34-A709-A1B3C21EF1FA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1703010F-427F-4A34-A709-A1B3C21EF1FA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="157">
   <si>
     <t>Number</t>
   </si>
@@ -302,30 +302,6 @@
     <t>Spring</t>
   </si>
   <si>
-    <t>S04</t>
-  </si>
-  <si>
-    <t>Urea</t>
-  </si>
-  <si>
-    <t>S11</t>
-  </si>
-  <si>
-    <t>S16</t>
-  </si>
-  <si>
-    <t>S22</t>
-  </si>
-  <si>
-    <t>W01</t>
-  </si>
-  <si>
-    <t>W38</t>
-  </si>
-  <si>
-    <t>W39</t>
-  </si>
-  <si>
     <t>S47</t>
   </si>
   <si>
@@ -399,16 +375,148 @@
   </si>
   <si>
     <t>Butyrate</t>
+  </si>
+  <si>
+    <t>W40</t>
+  </si>
+  <si>
+    <t>W41</t>
+  </si>
+  <si>
+    <t>W42</t>
+  </si>
+  <si>
+    <t>W43</t>
+  </si>
+  <si>
+    <t>W44</t>
+  </si>
+  <si>
+    <t>W45</t>
+  </si>
+  <si>
+    <t>W46</t>
+  </si>
+  <si>
+    <t>W47</t>
+  </si>
+  <si>
+    <t>W48</t>
+  </si>
+  <si>
+    <t>W50</t>
+  </si>
+  <si>
+    <t>W51</t>
+  </si>
+  <si>
+    <t>W57</t>
+  </si>
+  <si>
+    <t>W63</t>
+  </si>
+  <si>
+    <t>W66</t>
+  </si>
+  <si>
+    <t>W67</t>
+  </si>
+  <si>
+    <t>W68</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P18</t>
+  </si>
+  <si>
+    <t>P19</t>
+  </si>
+  <si>
+    <t>P20</t>
+  </si>
+  <si>
+    <t>P21</t>
+  </si>
+  <si>
+    <t>P22</t>
+  </si>
+  <si>
+    <t>P23</t>
+  </si>
+  <si>
+    <t>P24</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>P26</t>
+  </si>
+  <si>
+    <t>P27</t>
+  </si>
+  <si>
+    <t>P28</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>P30</t>
+  </si>
+  <si>
+    <t>P31</t>
+  </si>
+  <si>
+    <t>P32</t>
+  </si>
+  <si>
+    <t>P33</t>
+  </si>
+  <si>
+    <t>P34</t>
+  </si>
+  <si>
+    <t>P35</t>
+  </si>
+  <si>
+    <t>P36</t>
+  </si>
+  <si>
+    <t>P37</t>
+  </si>
+  <si>
+    <t>P38</t>
+  </si>
+  <si>
+    <t>P39</t>
+  </si>
+  <si>
+    <t>P40</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>P46</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -756,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9715411-D9A2-427F-BF3E-80D304B834E6}">
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:XFD152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -849,30 +957,30 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3995</v>
+        <v>4022</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4022</v>
+        <v>3991</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>68</v>
@@ -884,21 +992,21 @@
         <v>8</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>3991</v>
+        <v>4016</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -909,10 +1017,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>4016</v>
+        <v>4029</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>68</v>
@@ -924,15 +1032,15 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>4029</v>
+        <v>3992</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>68</v>
@@ -941,38 +1049,38 @@
         <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>3992</v>
+        <v>3967</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>4026</v>
+        <v>4031</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>68</v>
@@ -984,15 +1092,15 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>3967</v>
+        <v>4044</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>68</v>
@@ -1001,27 +1109,27 @@
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>4031</v>
+        <v>3966</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>70</v>
@@ -1029,10 +1137,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>4044</v>
+        <v>3983</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>68</v>
@@ -1041,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>70</v>
@@ -1049,10 +1157,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>3978</v>
+        <v>4045</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>68</v>
@@ -1064,35 +1172,35 @@
         <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>3966</v>
+        <v>4002</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>3983</v>
+        <v>4043</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>68</v>
@@ -1101,58 +1209,58 @@
         <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>4045</v>
+        <v>4030</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>4032</v>
+        <v>4037</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>4002</v>
+        <v>4000</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>68</v>
@@ -1161,18 +1269,18 @@
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>4043</v>
+        <v>4010</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>68</v>
@@ -1181,58 +1289,58 @@
         <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>4030</v>
+        <v>4038</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>4037</v>
+        <v>4036</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>4000</v>
+        <v>4007</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>68</v>
@@ -1249,70 +1357,70 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>4010</v>
+        <v>3973</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>4038</v>
+        <v>4008</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>4036</v>
+        <v>3982</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>4007</v>
+        <v>4019</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>68</v>
@@ -1321,18 +1429,18 @@
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>3973</v>
+        <v>4126</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>68</v>
@@ -1341,18 +1449,18 @@
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>4008</v>
+        <v>4142</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>68</v>
@@ -1364,15 +1472,15 @@
         <v>8</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>3982</v>
+        <v>4134</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>68</v>
@@ -1381,7 +1489,7 @@
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>9</v>
@@ -1389,371 +1497,375 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>4019</v>
+        <v>4154</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>4126</v>
+        <v>4105</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>4160</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>4081</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>4097</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>4171</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>4142</v>
-      </c>
-      <c r="B34" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>4089</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>4134</v>
-      </c>
-      <c r="B35" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>4084</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>4154</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="C39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>4185</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>4105</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>4143</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>4160</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C41" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>4169</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>4081</v>
-      </c>
-      <c r="B39" s="1" t="s">
+      <c r="C42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>4106</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>4097</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="C43" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>4138</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>4171</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>4158</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>4089</v>
-      </c>
-      <c r="B42" s="1" t="s">
+      <c r="C45" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>4166</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>4084</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="C46" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>4103</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>4185</v>
-      </c>
-      <c r="B44" s="1" t="s">
+      <c r="C47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>4184</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>4143</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>4169</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>4106</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>4138</v>
-      </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
-        <v>4158</v>
+        <v>4112</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
-        <v>4166</v>
+        <v>4066</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>68</v>
@@ -1762,124 +1874,120 @@
         <v>10</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G50" s="2"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
-        <v>4103</v>
+        <v>4067</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G51" s="2"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="2">
-        <v>4184</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G52" s="2"/>
+      <c r="A52" s="1">
+        <v>4013</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="2">
-        <v>4112</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="2"/>
+      <c r="A53" s="1">
+        <v>4056</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="2">
-        <v>4066</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G54" s="2"/>
+      <c r="A54" s="1">
+        <v>4005</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="2">
-        <v>4067</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="G55" s="2"/>
+      <c r="A55" s="1">
+        <v>4040</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>4034</v>
+        <v>3986</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>95</v>
+        <v>43</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>7</v>
@@ -1891,35 +1999,35 @@
         <v>71</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>4013</v>
+        <v>3996</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>4056</v>
+        <v>4047</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>7</v>
@@ -1931,15 +2039,15 @@
         <v>71</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>4005</v>
+        <v>3971</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>7</v>
@@ -1956,10 +2064,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>4040</v>
+        <v>4028</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>7</v>
@@ -1976,10 +2084,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>3986</v>
+        <v>4006</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>7</v>
@@ -1991,41 +2099,41 @@
         <v>71</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>3996</v>
+        <v>4042</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>4047</v>
+        <v>3979</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>71</v>
@@ -2036,36 +2144,36 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>3971</v>
+        <v>4035</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>4028</v>
+        <v>4048</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>71</v>
@@ -2076,10 +2184,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>4006</v>
+        <v>3997</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>7</v>
@@ -2088,27 +2196,27 @@
         <v>10</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>4042</v>
+        <v>4011</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>69</v>
@@ -2116,70 +2224,70 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>3979</v>
+        <v>3970</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>4035</v>
+        <v>3969</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>4048</v>
+        <v>4041</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>3997</v>
+        <v>3976</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>7</v>
@@ -2196,30 +2304,30 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>4011</v>
+        <v>4039</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>3970</v>
+        <v>3974</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
@@ -2231,15 +2339,15 @@
         <v>8</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>3969</v>
+        <v>4021</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>7</v>
@@ -2256,10 +2364,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>4041</v>
+        <v>3980</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>7</v>
@@ -2276,10 +2384,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>3976</v>
+        <v>4054</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>7</v>
@@ -2291,15 +2399,15 @@
         <v>8</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>4039</v>
+        <v>3989</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>7</v>
@@ -2311,15 +2419,15 @@
         <v>8</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>3974</v>
+        <v>4050</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>7</v>
@@ -2331,15 +2439,15 @@
         <v>8</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>4021</v>
+        <v>3975</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>7</v>
@@ -2351,15 +2459,15 @@
         <v>8</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>3980</v>
+        <v>4014</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>7</v>
@@ -2371,15 +2479,15 @@
         <v>8</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>4054</v>
+        <v>4017</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>7</v>
@@ -2391,55 +2499,55 @@
         <v>8</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>3989</v>
+        <v>4004</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>4050</v>
+        <v>4162</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>3975</v>
+        <v>4152</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>7</v>
@@ -2456,39 +2564,39 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>4014</v>
+        <v>4161</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>4017</v>
+        <v>4172</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>69</v>
@@ -2496,99 +2604,99 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>4004</v>
+        <v>4173</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>4003</v>
+        <v>4125</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>4055</v>
+        <v>4188</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>3998</v>
+        <v>4117</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>3968</v>
+        <v>4079</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>70</v>
@@ -2596,19 +2704,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>3987</v>
+        <v>4148</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>75</v>
+        <v>124</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>69</v>
@@ -2616,113 +2724,113 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>3957</v>
+        <v>4115</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>4023</v>
+        <v>4179</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>71</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>3993</v>
+        <v>4087</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>69</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>4033</v>
+        <v>4141</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>3985</v>
+        <v>4104</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>80</v>
+        <v>129</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>3999</v>
+        <v>4163</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>11</v>
@@ -2731,15 +2839,15 @@
         <v>8</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>3984</v>
+        <v>3998</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>89</v>
@@ -2751,35 +2859,35 @@
         <v>8</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>3990</v>
+        <v>3968</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
-        <v>4012</v>
+        <v>3987</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>89</v>
@@ -2796,85 +2904,786 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>4015</v>
+        <v>3957</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>4053</v>
+        <v>4023</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
-        <v>4025</v>
+        <v>3993</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>89</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
+        <v>4033</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>3985</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>3999</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>3984</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>3990</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>4012</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>4015</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>4053</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>4025</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
         <v>4046</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>69</v>
+      <c r="C114" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>4178</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>4144</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>4119</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>4130</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>4128</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>4108</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>4149</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>4150</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>4170</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>4085</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>4177</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>4127</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
+        <v>4139</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
+        <v>4090</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
+        <v>4113</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F129" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
+        <v>4116</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
+        <v>4095</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F131" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
+        <v>4155</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
+        <v>4110</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
+        <v>4118</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
+        <v>4135</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
+        <v>4167</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F136" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
+        <v>4146</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="1">
+        <v>4078</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1">
+        <v>4098</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="1">
+        <v>4096</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed metadata mix-up btwn inulin/saline no abx winter; updated stats; updated plots
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\CRDS_Calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9FAF145-0EBC-457E-8282-494011A72767}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2595D370-2854-45C9-93ED-EFCB70C936FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1703010F-427F-4A34-A709-A1B3C21EF1FA}"/>
   </bookViews>
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9715411-D9A2-427F-BF3E-80D304B834E6}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141:XFD152"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2559,7 +2559,7 @@
         <v>8</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added in missed sample (no CRDS but yes 16S)
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2FAD78D-5321-4650-8F66-CC81F1109CB4}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA2238B-C940-4B7F-BE67-9603699FCE13}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="110">
   <si>
     <t>Number</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>S11</t>
   </si>
 </sst>
 </file>
@@ -1198,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2576,19 +2579,19 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3967</v>
+        <v>4026</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
@@ -2596,17 +2599,11 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37">
-        <v>3958</v>
-      </c>
-      <c r="I37" t="s">
-        <v>102</v>
-      </c>
       <c r="J37">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="K37">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L37" t="s">
         <v>108</v>
@@ -2614,37 +2611,37 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>4045</v>
+        <v>3967</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>3954</v>
+        <v>3958</v>
       </c>
       <c r="I38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J38">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="K38">
-        <v>38.5</v>
+        <v>35</v>
       </c>
       <c r="L38" t="s">
         <v>108</v>
@@ -2652,10 +2649,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>4002</v>
+        <v>4045</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -2667,22 +2664,22 @@
         <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39">
-        <v>3955</v>
+        <v>3954</v>
       </c>
       <c r="I39" t="s">
         <v>103</v>
       </c>
       <c r="J39">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="K39">
-        <v>34</v>
+        <v>38.5</v>
       </c>
       <c r="L39" t="s">
         <v>108</v>
@@ -2690,19 +2687,19 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>4043</v>
+        <v>4002</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -2711,16 +2708,16 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>3954</v>
+        <v>3955</v>
       </c>
       <c r="I40" t="s">
         <v>103</v>
       </c>
       <c r="J40">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="K40">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L40" t="s">
         <v>108</v>
@@ -2728,37 +2725,37 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>4000</v>
+        <v>4043</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41">
-        <v>3955</v>
+        <v>3954</v>
       </c>
       <c r="I41" t="s">
         <v>103</v>
       </c>
       <c r="J41">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="K41">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L41" t="s">
         <v>108</v>
@@ -2766,19 +2763,19 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>4010</v>
+        <v>4000</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -2787,16 +2784,16 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>3957</v>
+        <v>3955</v>
       </c>
       <c r="I42" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J42">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="K42">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L42" t="s">
         <v>108</v>
@@ -2804,37 +2801,37 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>4038</v>
+        <v>4010</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>3956</v>
+        <v>3957</v>
       </c>
       <c r="I43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J43">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="K43">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L43" t="s">
         <v>108</v>
@@ -2842,10 +2839,10 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>4036</v>
+        <v>4038</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -2854,7 +2851,7 @@
         <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -2869,10 +2866,10 @@
         <v>103</v>
       </c>
       <c r="J44">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K44">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L44" t="s">
         <v>108</v>
@@ -2880,10 +2877,10 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>4007</v>
+        <v>4036</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -2895,22 +2892,22 @@
         <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45">
-        <v>3957</v>
+        <v>3956</v>
       </c>
       <c r="I45" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J45">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K45">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L45" t="s">
         <v>108</v>
@@ -2918,19 +2915,19 @@
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>3982</v>
+        <v>4007</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -2939,16 +2936,16 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>3961</v>
+        <v>3957</v>
       </c>
       <c r="I46" t="s">
         <v>102</v>
       </c>
       <c r="J46">
-        <v>158</v>
+        <v>213</v>
       </c>
       <c r="K46">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L46" t="s">
         <v>108</v>
@@ -2956,37 +2953,37 @@
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>4019</v>
+        <v>3982</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47">
-        <v>3947</v>
+        <v>3961</v>
       </c>
       <c r="I47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J47">
-        <v>211</v>
+        <v>158</v>
       </c>
       <c r="K47">
-        <v>33.5</v>
+        <v>35</v>
       </c>
       <c r="L47" t="s">
         <v>108</v>
@@ -2994,10 +2991,10 @@
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>4126</v>
+        <v>4019</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
@@ -3006,42 +3003,42 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
       </c>
       <c r="G48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H48">
-        <v>4065</v>
+        <v>3947</v>
       </c>
       <c r="I48" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J48">
-        <v>162</v>
+        <v>211</v>
       </c>
       <c r="K48">
-        <v>36</v>
-      </c>
-      <c r="L48">
-        <v>0.6</v>
+        <v>33.5</v>
+      </c>
+      <c r="L48" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>4142</v>
+        <v>4126</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -3053,27 +3050,27 @@
         <v>2</v>
       </c>
       <c r="H49">
-        <v>4061</v>
+        <v>4065</v>
       </c>
       <c r="I49" t="s">
         <v>102</v>
       </c>
       <c r="J49">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="K49">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L49">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>4134</v>
+        <v>4142</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -3085,33 +3082,33 @@
         <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G50">
         <v>2</v>
       </c>
       <c r="H50">
-        <v>4076</v>
+        <v>4061</v>
       </c>
       <c r="I50" t="s">
         <v>102</v>
       </c>
       <c r="J50">
-        <v>147.6</v>
+        <v>143</v>
       </c>
       <c r="K50">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L50">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>4154</v>
+        <v>4134</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -3129,16 +3126,16 @@
         <v>2</v>
       </c>
       <c r="H51">
-        <v>4062</v>
+        <v>4076</v>
       </c>
       <c r="I51" t="s">
         <v>102</v>
       </c>
       <c r="J51">
-        <v>167.1</v>
+        <v>147.6</v>
       </c>
       <c r="K51">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="L51">
         <v>0.6</v>
@@ -3146,37 +3143,37 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>4081</v>
+        <v>4154</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G52">
         <v>2</v>
       </c>
       <c r="H52">
-        <v>4072</v>
+        <v>4062</v>
       </c>
       <c r="I52" t="s">
         <v>102</v>
       </c>
       <c r="J52">
-        <v>160.80000000000001</v>
+        <v>167.1</v>
       </c>
       <c r="K52">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L52">
         <v>0.6</v>
@@ -3184,10 +3181,10 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>4097</v>
+        <v>4081</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -3205,33 +3202,33 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>4067</v>
+        <v>4072</v>
       </c>
       <c r="I53" t="s">
         <v>102</v>
       </c>
       <c r="J53">
-        <v>159.19999999999999</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="K53">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L53">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>4089</v>
+        <v>4097</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E54" t="s">
         <v>20</v>
@@ -3243,71 +3240,71 @@
         <v>2</v>
       </c>
       <c r="H54">
-        <v>4064</v>
+        <v>4067</v>
       </c>
       <c r="I54" t="s">
         <v>102</v>
       </c>
       <c r="J54">
-        <v>166.2</v>
+        <v>159.19999999999999</v>
       </c>
       <c r="K54">
         <v>37</v>
       </c>
       <c r="L54">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>4143</v>
+        <v>4089</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G55">
         <v>2</v>
       </c>
       <c r="H55">
-        <v>4061</v>
+        <v>4064</v>
       </c>
       <c r="I55" t="s">
         <v>102</v>
       </c>
       <c r="J55">
-        <v>159.1</v>
+        <v>166.2</v>
       </c>
       <c r="K55">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L55">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>4169</v>
+        <v>4143</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
         <v>20</v>
@@ -3319,33 +3316,33 @@
         <v>2</v>
       </c>
       <c r="H56">
-        <v>4063</v>
+        <v>4061</v>
       </c>
       <c r="I56" t="s">
         <v>102</v>
       </c>
       <c r="J56">
-        <v>162</v>
+        <v>159.1</v>
       </c>
       <c r="K56">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L56">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>4106</v>
+        <v>4169</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
@@ -3357,16 +3354,16 @@
         <v>2</v>
       </c>
       <c r="H57">
-        <v>4066</v>
+        <v>4063</v>
       </c>
       <c r="I57" t="s">
         <v>102</v>
       </c>
       <c r="J57">
-        <v>152.1</v>
+        <v>162</v>
       </c>
       <c r="K57">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="L57">
         <v>0.2</v>
@@ -3374,13 +3371,13 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>4013</v>
+        <v>4106</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3392,68 +3389,68 @@
         <v>14</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H58">
-        <v>3957</v>
+        <v>4066</v>
       </c>
       <c r="I58" t="s">
         <v>102</v>
       </c>
       <c r="J58">
-        <v>125.4</v>
+        <v>152.1</v>
       </c>
       <c r="K58">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L58">
-        <v>1.6</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>4056</v>
+        <v>4013</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C59" t="s">
         <v>43</v>
       </c>
       <c r="D59" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="H59">
-        <v>3945</v>
+        <v>3957</v>
       </c>
       <c r="I59" t="s">
         <v>102</v>
       </c>
       <c r="J59">
-        <v>157.5</v>
+        <v>125.4</v>
       </c>
       <c r="K59">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L59">
-        <v>2.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>4040</v>
+        <v>4056</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C60" t="s">
         <v>43</v>
@@ -3465,22 +3462,22 @@
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60">
-        <v>3956</v>
+        <v>3945</v>
       </c>
       <c r="I60" t="s">
         <v>102</v>
       </c>
       <c r="J60">
-        <v>153.9</v>
+        <v>157.5</v>
       </c>
       <c r="K60">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="L60">
         <v>2.4</v>
@@ -3488,92 +3485,92 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>3986</v>
+        <v>4040</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61">
-        <v>3961</v>
+        <v>3956</v>
       </c>
       <c r="I61" t="s">
         <v>102</v>
       </c>
       <c r="J61">
-        <v>142</v>
+        <v>153.9</v>
       </c>
       <c r="K61">
-        <v>38</v>
+        <v>36.5</v>
       </c>
       <c r="L61">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>4028</v>
+        <v>3986</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C62" t="s">
         <v>43</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
       <c r="H62">
-        <v>3946</v>
+        <v>3961</v>
       </c>
       <c r="I62" t="s">
         <v>102</v>
       </c>
       <c r="J62">
-        <v>133.80000000000001</v>
+        <v>142</v>
       </c>
       <c r="K62">
         <v>38</v>
       </c>
       <c r="L62">
-        <v>2.8</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>4006</v>
+        <v>4028</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C63" t="s">
         <v>43</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
@@ -3585,27 +3582,27 @@
         <v>1</v>
       </c>
       <c r="H63">
-        <v>3955</v>
+        <v>3946</v>
       </c>
       <c r="I63" t="s">
         <v>102</v>
       </c>
       <c r="J63">
-        <v>134.9</v>
+        <v>133.80000000000001</v>
       </c>
       <c r="K63">
-        <v>37.5</v>
+        <v>38</v>
       </c>
       <c r="L63">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>4042</v>
+        <v>4006</v>
       </c>
       <c r="B64" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C64" t="s">
         <v>43</v>
@@ -3617,39 +3614,39 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="H64">
-        <v>3956</v>
+        <v>3955</v>
       </c>
       <c r="I64" t="s">
         <v>102</v>
       </c>
       <c r="J64">
-        <v>137.30000000000001</v>
+        <v>134.9</v>
       </c>
       <c r="K64">
         <v>37.5</v>
       </c>
       <c r="L64">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>4035</v>
+        <v>4042</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C65" t="s">
         <v>43</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
         <v>20</v>
@@ -3661,65 +3658,65 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>3949</v>
+        <v>3956</v>
       </c>
       <c r="I65" t="s">
         <v>102</v>
       </c>
       <c r="J65">
-        <v>150.30000000000001</v>
+        <v>137.30000000000001</v>
       </c>
       <c r="K65">
-        <v>38</v>
+        <v>37.5</v>
       </c>
       <c r="L65">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>4048</v>
+        <v>4035</v>
       </c>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C66" t="s">
         <v>43</v>
       </c>
       <c r="D66" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
       <c r="H66">
-        <v>3954</v>
+        <v>3949</v>
       </c>
       <c r="I66" t="s">
         <v>102</v>
       </c>
       <c r="J66">
-        <v>134.19999999999999</v>
+        <v>150.30000000000001</v>
       </c>
       <c r="K66">
         <v>38</v>
       </c>
       <c r="L66">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>3997</v>
+        <v>4048</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C67" t="s">
         <v>43</v>
@@ -3728,42 +3725,42 @@
         <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G67">
         <v>1</v>
       </c>
       <c r="H67">
-        <v>3948</v>
+        <v>3954</v>
       </c>
       <c r="I67" t="s">
         <v>102</v>
       </c>
       <c r="J67">
-        <v>128.6</v>
+        <v>134.19999999999999</v>
       </c>
       <c r="K67">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L67">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>4011</v>
+        <v>3997</v>
       </c>
       <c r="B68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C68" t="s">
         <v>43</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -3775,27 +3772,27 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>3957</v>
+        <v>3948</v>
       </c>
       <c r="I68" t="s">
         <v>102</v>
       </c>
       <c r="J68">
-        <v>141.80000000000001</v>
+        <v>128.6</v>
       </c>
       <c r="K68">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="L68">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>3970</v>
+        <v>4011</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C69" t="s">
         <v>43</v>
@@ -3813,16 +3810,16 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>3958</v>
+        <v>3957</v>
       </c>
       <c r="I69" t="s">
         <v>102</v>
       </c>
       <c r="J69">
-        <v>185.8</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="K69">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L69">
         <v>1.2</v>
@@ -3830,16 +3827,16 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3976</v>
+        <v>3970</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
         <v>43</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -3851,27 +3848,27 @@
         <v>1</v>
       </c>
       <c r="H70">
-        <v>3959</v>
+        <v>3958</v>
       </c>
       <c r="I70" t="s">
         <v>102</v>
       </c>
       <c r="J70">
-        <v>114</v>
+        <v>185.8</v>
       </c>
       <c r="K70">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L70">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>4054</v>
+        <v>3976</v>
       </c>
       <c r="B71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C71" t="s">
         <v>43</v>
@@ -3883,33 +3880,33 @@
         <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G71">
         <v>1</v>
       </c>
       <c r="H71">
-        <v>3945</v>
+        <v>3959</v>
       </c>
       <c r="I71" t="s">
         <v>102</v>
       </c>
       <c r="J71">
-        <v>116.5</v>
+        <v>114</v>
       </c>
       <c r="K71">
-        <v>37.5</v>
+        <v>36.5</v>
       </c>
       <c r="L71">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>3989</v>
+        <v>4054</v>
       </c>
       <c r="B72" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C72" t="s">
         <v>43</v>
@@ -3927,33 +3924,33 @@
         <v>1</v>
       </c>
       <c r="H72">
-        <v>3961</v>
+        <v>3945</v>
       </c>
       <c r="I72" t="s">
         <v>102</v>
       </c>
       <c r="J72">
-        <v>126.3</v>
+        <v>116.5</v>
       </c>
       <c r="K72">
-        <v>38</v>
+        <v>37.5</v>
       </c>
       <c r="L72">
-        <v>3.9</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>4050</v>
+        <v>3989</v>
       </c>
       <c r="B73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C73" t="s">
         <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -3965,33 +3962,33 @@
         <v>1</v>
       </c>
       <c r="H73">
-        <v>3954</v>
+        <v>3961</v>
       </c>
       <c r="I73" t="s">
         <v>102</v>
       </c>
       <c r="J73">
-        <v>141.30000000000001</v>
+        <v>126.3</v>
       </c>
       <c r="K73">
         <v>38</v>
       </c>
       <c r="L73">
-        <v>1.5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>3975</v>
+        <v>4050</v>
       </c>
       <c r="B74" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C74" t="s">
         <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -4003,33 +4000,33 @@
         <v>1</v>
       </c>
       <c r="H74">
-        <v>3959</v>
+        <v>3954</v>
       </c>
       <c r="I74" t="s">
         <v>102</v>
       </c>
       <c r="J74">
-        <v>116.6</v>
+        <v>141.30000000000001</v>
       </c>
       <c r="K74">
-        <v>35.5</v>
+        <v>38</v>
       </c>
       <c r="L74">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>4014</v>
+        <v>3975</v>
       </c>
       <c r="B75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C75" t="s">
         <v>43</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -4041,71 +4038,71 @@
         <v>1</v>
       </c>
       <c r="H75">
-        <v>3957</v>
+        <v>3959</v>
       </c>
       <c r="I75" t="s">
         <v>102</v>
       </c>
       <c r="J75">
-        <v>138.1</v>
+        <v>116.6</v>
       </c>
       <c r="K75">
         <v>35.5</v>
       </c>
       <c r="L75">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>4017</v>
+        <v>4014</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C76" t="s">
         <v>43</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
       </c>
       <c r="F76" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G76">
         <v>1</v>
       </c>
       <c r="H76">
-        <v>3947</v>
+        <v>3957</v>
       </c>
       <c r="I76" t="s">
         <v>102</v>
       </c>
       <c r="J76">
-        <v>133.6</v>
+        <v>138.1</v>
       </c>
       <c r="K76">
-        <v>37</v>
+        <v>35.5</v>
       </c>
       <c r="L76">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>4004</v>
+        <v>4017</v>
       </c>
       <c r="B77" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
         <v>43</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -4117,33 +4114,33 @@
         <v>1</v>
       </c>
       <c r="H77">
-        <v>3955</v>
+        <v>3947</v>
       </c>
       <c r="I77" t="s">
         <v>102</v>
       </c>
       <c r="J77">
-        <v>134.6</v>
+        <v>133.6</v>
       </c>
       <c r="K77">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L77">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>4152</v>
+        <v>4004</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C78" t="s">
         <v>43</v>
       </c>
       <c r="D78" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -4152,30 +4149,30 @@
         <v>11</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78">
-        <v>4063</v>
+        <v>3955</v>
       </c>
       <c r="I78" t="s">
         <v>102</v>
       </c>
       <c r="J78">
-        <v>101.5</v>
+        <v>134.6</v>
       </c>
       <c r="K78">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L78">
-        <v>5.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>4161</v>
+        <v>4152</v>
       </c>
       <c r="B79" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
         <v>43</v>
@@ -4184,86 +4181,86 @@
         <v>12</v>
       </c>
       <c r="E79" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F79" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G79">
         <v>2</v>
       </c>
       <c r="H79">
-        <v>4062</v>
+        <v>4063</v>
       </c>
       <c r="I79" t="s">
         <v>102</v>
       </c>
       <c r="J79">
-        <v>115.8</v>
+        <v>101.5</v>
       </c>
       <c r="K79">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L79">
-        <v>2.2999999999999998</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>4172</v>
+        <v>4161</v>
       </c>
       <c r="B80" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C80" t="s">
         <v>43</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G80">
         <v>2</v>
       </c>
       <c r="H80">
-        <v>4064</v>
+        <v>4062</v>
       </c>
       <c r="I80" t="s">
         <v>102</v>
       </c>
       <c r="J80">
-        <v>157.19999999999999</v>
+        <v>115.8</v>
       </c>
       <c r="K80">
         <v>37</v>
       </c>
       <c r="L80">
-        <v>2.2000000000000002</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>4173</v>
+        <v>4172</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C81" t="s">
         <v>43</v>
       </c>
       <c r="D81" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F81" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G81">
         <v>2</v>
@@ -4275,21 +4272,21 @@
         <v>102</v>
       </c>
       <c r="J81">
-        <v>110.3</v>
+        <v>157.19999999999999</v>
       </c>
       <c r="K81">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="L81">
-        <v>2.7</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>4188</v>
+        <v>4173</v>
       </c>
       <c r="B82" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C82" t="s">
         <v>43</v>
@@ -4307,27 +4304,27 @@
         <v>2</v>
       </c>
       <c r="H82">
-        <v>4077</v>
+        <v>4064</v>
       </c>
       <c r="I82" t="s">
         <v>102</v>
       </c>
       <c r="J82">
-        <v>124.7</v>
+        <v>110.3</v>
       </c>
       <c r="K82">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L82">
-        <v>1.3</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>4117</v>
+        <v>4188</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
         <v>43</v>
@@ -4336,36 +4333,36 @@
         <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F83" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G83">
         <v>2</v>
       </c>
       <c r="H83">
-        <v>4070</v>
+        <v>4077</v>
       </c>
       <c r="I83" t="s">
         <v>102</v>
       </c>
       <c r="J83">
-        <v>132.5</v>
+        <v>124.7</v>
       </c>
       <c r="K83">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L83">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>4148</v>
+        <v>4117</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C84" t="s">
         <v>43</v>
@@ -4383,62 +4380,100 @@
         <v>2</v>
       </c>
       <c r="H84">
-        <v>4061</v>
+        <v>4070</v>
       </c>
       <c r="I84" t="s">
         <v>102</v>
       </c>
       <c r="J84">
-        <v>119.2</v>
+        <v>132.5</v>
       </c>
       <c r="K84">
-        <v>34.5</v>
+        <v>37</v>
       </c>
       <c r="L84">
-        <v>3.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>4115</v>
+        <v>4148</v>
       </c>
       <c r="B85" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
         <v>43</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G85">
         <v>2</v>
       </c>
       <c r="H85">
+        <v>4061</v>
+      </c>
+      <c r="I85" t="s">
+        <v>102</v>
+      </c>
+      <c r="J85">
+        <v>119.2</v>
+      </c>
+      <c r="K85">
+        <v>34.5</v>
+      </c>
+      <c r="L85">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>4115</v>
+      </c>
+      <c r="B86" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86" t="s">
+        <v>43</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86">
         <v>4066</v>
       </c>
-      <c r="I85" t="s">
-        <v>102</v>
-      </c>
-      <c r="J85">
+      <c r="I86" t="s">
+        <v>102</v>
+      </c>
+      <c r="J86">
         <v>121.6</v>
       </c>
-      <c r="K85">
+      <c r="K86">
         <v>34</v>
       </c>
-      <c r="L85">
+      <c r="L86">
         <v>2.2000000000000002</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L85">
-    <sortCondition ref="B1:B85"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L86">
+    <sortCondition ref="B1:B86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added date sampled; changed .csv type
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A5C03FC-20FD-4CD2-A35B-24C8F7BE8EDF}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DB7BBD4-C131-4982-BC47-F7900186AFE0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="111">
   <si>
     <t>Number</t>
   </si>
@@ -361,6 +361,9 @@
   </si>
   <si>
     <t>S11</t>
+  </si>
+  <si>
+    <t>Date_Sampled</t>
   </si>
 </sst>
 </file>
@@ -844,8 +847,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1201,15 +1211,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
+      <selection activeCell="N57" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="13" max="13" width="14" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,8 +1259,11 @@
       <c r="L1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3998</v>
       </c>
@@ -1284,8 +1300,11 @@
       <c r="L2">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" s="3">
+        <v>43167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3987</v>
       </c>
@@ -1322,8 +1341,11 @@
       <c r="L3">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="3">
+        <v>43171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3957</v>
       </c>
@@ -1360,8 +1382,11 @@
       <c r="L4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="3">
+        <v>43174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4023</v>
       </c>
@@ -1398,8 +1423,11 @@
       <c r="L5">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="3">
+        <v>43175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3993</v>
       </c>
@@ -1436,8 +1464,11 @@
       <c r="L6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="3">
+        <v>43178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4033</v>
       </c>
@@ -1474,8 +1505,11 @@
       <c r="L7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="3">
+        <v>43179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3985</v>
       </c>
@@ -1512,8 +1546,11 @@
       <c r="L8">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="3">
+        <v>43180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3999</v>
       </c>
@@ -1550,8 +1587,11 @@
       <c r="L9">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="3">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3990</v>
       </c>
@@ -1588,8 +1628,11 @@
       <c r="L10">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="3">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4012</v>
       </c>
@@ -1626,8 +1669,11 @@
       <c r="L11">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="3">
+        <v>43186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4025</v>
       </c>
@@ -1664,8 +1710,11 @@
       <c r="L12">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="3">
+        <v>43188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4046</v>
       </c>
@@ -1702,8 +1751,11 @@
       <c r="L13">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="3">
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4119</v>
       </c>
@@ -1740,8 +1792,11 @@
       <c r="L14">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="3">
+        <v>43536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4130</v>
       </c>
@@ -1778,8 +1833,11 @@
       <c r="L15">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="3">
+        <v>43536</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4128</v>
       </c>
@@ -1816,8 +1874,11 @@
       <c r="L16">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="3">
+        <v>43537</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4108</v>
       </c>
@@ -1854,8 +1915,11 @@
       <c r="L17">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="3">
+        <v>43537</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4150</v>
       </c>
@@ -1892,8 +1956,11 @@
       <c r="L18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="3">
+        <v>43538</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4085</v>
       </c>
@@ -1930,8 +1997,11 @@
       <c r="L19">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="3">
+        <v>43539</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4127</v>
       </c>
@@ -1968,8 +2038,11 @@
       <c r="L20">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="3">
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4090</v>
       </c>
@@ -2006,8 +2079,11 @@
       <c r="L21">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="3">
+        <v>43543</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4116</v>
       </c>
@@ -2044,8 +2120,11 @@
       <c r="L22">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="3">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>4095</v>
       </c>
@@ -2082,8 +2161,11 @@
       <c r="L23">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="3">
+        <v>43545</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4155</v>
       </c>
@@ -2120,8 +2202,11 @@
       <c r="L24">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="3">
+        <v>43545</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4110</v>
       </c>
@@ -2158,8 +2243,11 @@
       <c r="L25">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="3">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4118</v>
       </c>
@@ -2196,8 +2284,11 @@
       <c r="L26">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" s="3">
+        <v>43546</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4167</v>
       </c>
@@ -2234,8 +2325,11 @@
       <c r="L27">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" s="3">
+        <v>43549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4146</v>
       </c>
@@ -2272,8 +2366,11 @@
       <c r="L28">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" s="3">
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4098</v>
       </c>
@@ -2310,8 +2407,11 @@
       <c r="L29">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="3">
+        <v>43551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3964</v>
       </c>
@@ -2348,8 +2448,11 @@
       <c r="L30" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="1">
+        <v>42929</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3981</v>
       </c>
@@ -2386,8 +2489,11 @@
       <c r="L31" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" s="3">
+        <v>42935</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4022</v>
       </c>
@@ -2424,8 +2530,11 @@
       <c r="L32" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" s="3">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3991</v>
       </c>
@@ -2462,8 +2571,11 @@
       <c r="L33" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" s="3">
+        <v>42942</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4016</v>
       </c>
@@ -2500,8 +2612,11 @@
       <c r="L34" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" s="3">
+        <v>42943</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4029</v>
       </c>
@@ -2538,8 +2653,11 @@
       <c r="L35" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="3">
+        <v>42944</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3992</v>
       </c>
@@ -2576,8 +2694,11 @@
       <c r="L36" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="3">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4026</v>
       </c>
@@ -2614,8 +2735,11 @@
       <c r="L37" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="3">
+        <v>42949</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3967</v>
       </c>
@@ -2652,8 +2776,11 @@
       <c r="L38" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" s="3">
+        <v>42950</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4045</v>
       </c>
@@ -2690,8 +2817,11 @@
       <c r="L39" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" s="3">
+        <v>42961</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4002</v>
       </c>
@@ -2728,8 +2858,11 @@
       <c r="L40" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40" s="3">
+        <v>42963</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4043</v>
       </c>
@@ -2766,8 +2899,11 @@
       <c r="L41" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41" s="3">
+        <v>42964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>4000</v>
       </c>
@@ -2804,8 +2940,11 @@
       <c r="L42" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M42" s="3">
+        <v>42970</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4010</v>
       </c>
@@ -2842,8 +2981,11 @@
       <c r="L43" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43" s="3">
+        <v>42971</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4038</v>
       </c>
@@ -2880,8 +3022,11 @@
       <c r="L44" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44" s="3">
+        <v>42972</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>4036</v>
       </c>
@@ -2918,8 +3063,11 @@
       <c r="L45" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45" s="3">
+        <v>42975</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4007</v>
       </c>
@@ -2956,8 +3104,11 @@
       <c r="L46" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M46" s="3">
+        <v>42977</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3982</v>
       </c>
@@ -2994,8 +3145,11 @@
       <c r="L47" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47" s="3">
+        <v>42979</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>4019</v>
       </c>
@@ -3032,8 +3186,11 @@
       <c r="L48" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" s="3">
+        <v>42983</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4126</v>
       </c>
@@ -3070,8 +3227,11 @@
       <c r="L49">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49" s="3">
+        <v>43322</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4142</v>
       </c>
@@ -3108,8 +3268,11 @@
       <c r="L50">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50" s="3">
+        <v>43322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4134</v>
       </c>
@@ -3146,8 +3309,11 @@
       <c r="L51">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51" s="3">
+        <v>43325</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>4154</v>
       </c>
@@ -3184,8 +3350,11 @@
       <c r="L52">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52" s="3">
+        <v>43325</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4081</v>
       </c>
@@ -3222,8 +3391,11 @@
       <c r="L53">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53" s="3">
+        <v>43327</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4097</v>
       </c>
@@ -3260,8 +3432,11 @@
       <c r="L54">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54" s="3">
+        <v>43327</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4089</v>
       </c>
@@ -3298,8 +3473,11 @@
       <c r="L55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55" s="3">
+        <v>43328</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4143</v>
       </c>
@@ -3336,8 +3514,11 @@
       <c r="L56">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56" s="3">
+        <v>43332</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4169</v>
       </c>
@@ -3374,8 +3555,11 @@
       <c r="L57">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57" s="3">
+        <v>43332</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4106</v>
       </c>
@@ -3412,8 +3596,11 @@
       <c r="L58">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58" s="3">
+        <v>43333</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4013</v>
       </c>
@@ -3450,8 +3637,11 @@
       <c r="L59">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59" s="3">
+        <v>43122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4056</v>
       </c>
@@ -3488,8 +3678,11 @@
       <c r="L60">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60" s="3">
+        <v>43130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4040</v>
       </c>
@@ -3526,8 +3719,11 @@
       <c r="L61">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61" s="3">
+        <v>43129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>3986</v>
       </c>
@@ -3564,8 +3760,11 @@
       <c r="L62">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62" s="3">
+        <v>43131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4028</v>
       </c>
@@ -3602,8 +3801,11 @@
       <c r="L63">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63" s="3">
+        <v>43123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4006</v>
       </c>
@@ -3640,8 +3842,11 @@
       <c r="L64">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M64" s="3">
+        <v>43119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>4042</v>
       </c>
@@ -3678,8 +3883,11 @@
       <c r="L65">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65" s="3">
+        <v>43132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>4035</v>
       </c>
@@ -3716,8 +3924,11 @@
       <c r="L66">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66" s="3">
+        <v>43140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>4048</v>
       </c>
@@ -3754,8 +3965,11 @@
       <c r="L67">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67" s="3">
+        <v>43124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3997</v>
       </c>
@@ -3792,8 +4006,11 @@
       <c r="L68">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68" s="3">
+        <v>43146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>4011</v>
       </c>
@@ -3830,8 +4047,11 @@
       <c r="L69">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M69" s="3">
+        <v>43138</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3970</v>
       </c>
@@ -3868,8 +4088,11 @@
       <c r="L70">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70" s="3">
+        <v>43143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3976</v>
       </c>
@@ -3906,8 +4129,11 @@
       <c r="L71">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M71" s="3">
+        <v>43110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>4054</v>
       </c>
@@ -3944,8 +4170,11 @@
       <c r="L72">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72" s="3">
+        <v>43125</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3989</v>
       </c>
@@ -3982,8 +4211,11 @@
       <c r="L73">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M73" s="3">
+        <v>43126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>4050</v>
       </c>
@@ -4020,8 +4252,11 @@
       <c r="L74">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74" s="3">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3975</v>
       </c>
@@ -4058,8 +4293,11 @@
       <c r="L75">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M75" s="3">
+        <v>43136</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>4014</v>
       </c>
@@ -4096,8 +4334,11 @@
       <c r="L76">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76" s="3">
+        <v>43137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>4017</v>
       </c>
@@ -4134,8 +4375,11 @@
       <c r="L77">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77" s="3">
+        <v>43144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4004</v>
       </c>
@@ -4172,8 +4416,11 @@
       <c r="L78">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78" s="3">
+        <v>43145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>4152</v>
       </c>
@@ -4210,8 +4457,11 @@
       <c r="L79">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M79" s="3">
+        <v>43472</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>4161</v>
       </c>
@@ -4248,8 +4498,11 @@
       <c r="L80">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M80" s="3">
+        <v>43472</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4172</v>
       </c>
@@ -4286,8 +4539,11 @@
       <c r="L81">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M81" s="3">
+        <v>43473</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4173</v>
       </c>
@@ -4324,8 +4580,11 @@
       <c r="L82">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82" s="3">
+        <v>43473</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>4188</v>
       </c>
@@ -4362,8 +4621,11 @@
       <c r="L83">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M83" s="3">
+        <v>43474</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>4117</v>
       </c>
@@ -4400,8 +4662,11 @@
       <c r="L84">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" s="3">
+        <v>43475</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4148</v>
       </c>
@@ -4438,8 +4703,11 @@
       <c r="L85">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M85" s="3">
+        <v>43479</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4115</v>
       </c>
@@ -4475,6 +4743,9 @@
       </c>
       <c r="L86">
         <v>2.2000000000000002</v>
+      </c>
+      <c r="M86" s="3">
+        <v>43479</v>
       </c>
     </row>
   </sheetData>
@@ -4482,5 +4753,6 @@
     <sortCondition ref="B1:B86"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed P04 because adult
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DB7BBD4-C131-4982-BC47-F7900186AFE0}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B9461B1-3CE5-486A-B496-AC07F6C2E157}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="109">
   <si>
     <t>Number</t>
   </si>
@@ -255,9 +255,6 @@
     <t>P03</t>
   </si>
   <si>
-    <t>P04</t>
-  </si>
-  <si>
     <t>P05</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
   </si>
   <si>
     <t>P41</t>
-  </si>
-  <si>
-    <t>Adult</t>
   </si>
   <si>
     <t>Mom_Location</t>
@@ -1211,18 +1205,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M86"/>
+  <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B57" workbookViewId="0">
-      <selection activeCell="N57" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="14" style="2" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1245,25 +1241,26 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L1" t="s">
-        <v>107</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3998</v>
       </c>
@@ -1289,7 +1286,7 @@
         <v>3948</v>
       </c>
       <c r="I2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J2">
         <v>153.80000000000001</v>
@@ -1304,7 +1301,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3987</v>
       </c>
@@ -1330,7 +1327,7 @@
         <v>3961</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J3">
         <v>172.6</v>
@@ -1345,9 +1342,9 @@
         <v>43171</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3957</v>
+        <v>4023</v>
       </c>
       <c r="B4" t="s">
         <v>74</v>
@@ -1367,28 +1364,28 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>100</v>
+      <c r="H4">
+        <v>3946</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J4">
-        <v>143.6</v>
+        <v>170.3</v>
       </c>
       <c r="K4">
-        <v>37.5</v>
+        <v>39</v>
       </c>
       <c r="L4">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="M4" s="3">
-        <v>43174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4023</v>
+        <v>3993</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
@@ -1409,27 +1406,27 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>3946</v>
+        <v>3948</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J5">
-        <v>170.3</v>
+        <v>152.1</v>
       </c>
       <c r="K5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="L5">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="M5" s="3">
-        <v>43175</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3993</v>
+        <v>4033</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
@@ -1441,36 +1438,36 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>3948</v>
+        <v>3949</v>
       </c>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J6">
-        <v>152.1</v>
+        <v>154.6</v>
       </c>
       <c r="K6">
-        <v>40</v>
+        <v>38.5</v>
       </c>
       <c r="L6">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="M6" s="3">
-        <v>43178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4033</v>
+        <v>3985</v>
       </c>
       <c r="B7" t="s">
         <v>77</v>
@@ -1479,7 +1476,7 @@
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -1491,27 +1488,27 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>3949</v>
+        <v>3961</v>
       </c>
       <c r="I7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J7">
-        <v>154.6</v>
+        <v>170</v>
       </c>
       <c r="K7">
-        <v>38.5</v>
+        <v>39</v>
       </c>
       <c r="L7">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="M7" s="3">
-        <v>43179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3985</v>
+        <v>3999</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -1526,33 +1523,33 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>3961</v>
+        <v>3948</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J8">
-        <v>170</v>
+        <v>172.7</v>
       </c>
       <c r="K8">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L8">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="M8" s="3">
-        <v>43180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3999</v>
+        <v>3990</v>
       </c>
       <c r="B9" t="s">
         <v>79</v>
@@ -1567,33 +1564,33 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>3948</v>
+        <v>3961</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J9">
-        <v>172.7</v>
+        <v>188.6</v>
       </c>
       <c r="K9">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L9">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="M9" s="3">
-        <v>43181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3990</v>
+        <v>4012</v>
       </c>
       <c r="B10" t="s">
         <v>80</v>
@@ -1608,33 +1605,33 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>3961</v>
+        <v>3957</v>
       </c>
       <c r="I10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J10">
-        <v>188.6</v>
+        <v>170.1</v>
       </c>
       <c r="K10">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="M10" s="3">
-        <v>43185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4012</v>
+        <v>4025</v>
       </c>
       <c r="B11" t="s">
         <v>81</v>
@@ -1649,33 +1646,33 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>3957</v>
+        <v>3946</v>
       </c>
       <c r="I11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J11">
-        <v>170.1</v>
+        <v>159.6</v>
       </c>
       <c r="K11">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L11">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M11" s="3">
-        <v>43186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4025</v>
+        <v>4046</v>
       </c>
       <c r="B12" t="s">
         <v>82</v>
@@ -1690,33 +1687,33 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>3946</v>
+        <v>3954</v>
       </c>
       <c r="I12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J12">
-        <v>159.6</v>
+        <v>154.4</v>
       </c>
       <c r="K12">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L12">
         <v>0.2</v>
       </c>
       <c r="M12" s="3">
-        <v>43188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4046</v>
+        <v>4119</v>
       </c>
       <c r="B13" t="s">
         <v>83</v>
@@ -1728,36 +1725,36 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>3954</v>
+        <v>4070</v>
       </c>
       <c r="I13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J13">
-        <v>154.4</v>
+        <v>164.5</v>
       </c>
       <c r="K13">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L13">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="M13" s="3">
-        <v>43189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43536</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4119</v>
+        <v>4130</v>
       </c>
       <c r="B14" t="s">
         <v>84</v>
@@ -1766,7 +1763,7 @@
         <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
@@ -1778,27 +1775,27 @@
         <v>2</v>
       </c>
       <c r="H14">
-        <v>4070</v>
+        <v>4073</v>
       </c>
       <c r="I14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J14">
-        <v>164.5</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="K14">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L14">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="M14" s="3">
         <v>43536</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4130</v>
+        <v>4128</v>
       </c>
       <c r="B15" t="s">
         <v>85</v>
@@ -1813,7 +1810,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -1822,24 +1819,24 @@
         <v>4073</v>
       </c>
       <c r="I15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J15">
-        <v>149.80000000000001</v>
+        <v>130.5</v>
       </c>
       <c r="K15">
-        <v>36</v>
+        <v>37.5</v>
       </c>
       <c r="L15">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="M15" s="3">
-        <v>43536</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>43537</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4128</v>
+        <v>4108</v>
       </c>
       <c r="B16" t="s">
         <v>86</v>
@@ -1860,19 +1857,19 @@
         <v>2</v>
       </c>
       <c r="H16">
-        <v>4073</v>
+        <v>4066</v>
       </c>
       <c r="I16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J16">
-        <v>130.5</v>
+        <v>111.4</v>
       </c>
       <c r="K16">
-        <v>37.5</v>
+        <v>39</v>
       </c>
       <c r="L16">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="M16" s="3">
         <v>43537</v>
@@ -1880,7 +1877,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4108</v>
+        <v>4150</v>
       </c>
       <c r="B17" t="s">
         <v>87</v>
@@ -1889,39 +1886,39 @@
         <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17">
-        <v>4066</v>
+        <v>4061</v>
       </c>
       <c r="I17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J17">
-        <v>111.4</v>
+        <v>147.30000000000001</v>
       </c>
       <c r="K17">
         <v>39</v>
       </c>
       <c r="L17">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M17" s="3">
-        <v>43537</v>
+        <v>43538</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4150</v>
+        <v>4085</v>
       </c>
       <c r="B18" t="s">
         <v>88</v>
@@ -1936,33 +1933,33 @@
         <v>20</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="H18">
-        <v>4061</v>
+        <v>4069</v>
       </c>
       <c r="I18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J18">
-        <v>147.30000000000001</v>
+        <v>149.4</v>
       </c>
       <c r="K18">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L18">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="M18" s="3">
-        <v>43538</v>
+        <v>43539</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4085</v>
+        <v>4127</v>
       </c>
       <c r="B19" t="s">
         <v>89</v>
@@ -1983,27 +1980,27 @@
         <v>2</v>
       </c>
       <c r="H19">
-        <v>4069</v>
+        <v>4071</v>
       </c>
       <c r="I19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J19">
-        <v>149.4</v>
+        <v>118.9</v>
       </c>
       <c r="K19">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L19">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="M19" s="3">
-        <v>43539</v>
+        <v>43542</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4127</v>
+        <v>4090</v>
       </c>
       <c r="B20" t="s">
         <v>90</v>
@@ -2024,27 +2021,27 @@
         <v>2</v>
       </c>
       <c r="H20">
-        <v>4071</v>
+        <v>4068</v>
       </c>
       <c r="I20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J20">
-        <v>118.9</v>
+        <v>157.1</v>
       </c>
       <c r="K20">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L20">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="M20" s="3">
-        <v>43542</v>
+        <v>43543</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4090</v>
+        <v>4116</v>
       </c>
       <c r="B21" t="s">
         <v>91</v>
@@ -2059,33 +2056,33 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21">
-        <v>4068</v>
+        <v>4066</v>
       </c>
       <c r="I21" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J21">
-        <v>157.1</v>
+        <v>144.19999999999999</v>
       </c>
       <c r="K21">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L21">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M21" s="3">
-        <v>43543</v>
+        <v>43544</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4116</v>
+        <v>4095</v>
       </c>
       <c r="B22" t="s">
         <v>92</v>
@@ -2097,7 +2094,7 @@
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F22" t="s">
         <v>11</v>
@@ -2106,27 +2103,27 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>4066</v>
+        <v>4068</v>
       </c>
       <c r="I22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J22">
-        <v>144.19999999999999</v>
+        <v>170.9</v>
       </c>
       <c r="K22">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L22">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="M22" s="3">
-        <v>43544</v>
+        <v>43545</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4095</v>
+        <v>4155</v>
       </c>
       <c r="B23" t="s">
         <v>93</v>
@@ -2135,31 +2132,31 @@
         <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23">
-        <v>4068</v>
+        <v>4062</v>
       </c>
       <c r="I23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J23">
-        <v>170.9</v>
+        <v>134.6</v>
       </c>
       <c r="K23">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L23">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="M23" s="3">
         <v>43545</v>
@@ -2167,7 +2164,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4155</v>
+        <v>4110</v>
       </c>
       <c r="B24" t="s">
         <v>94</v>
@@ -2179,36 +2176,36 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="H24">
-        <v>4062</v>
+        <v>4066</v>
       </c>
       <c r="I24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J24">
-        <v>134.6</v>
+        <v>154.19999999999999</v>
       </c>
       <c r="K24">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L24">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="M24" s="3">
-        <v>43545</v>
+        <v>43546</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4110</v>
+        <v>4118</v>
       </c>
       <c r="B25" t="s">
         <v>95</v>
@@ -2223,22 +2220,22 @@
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="H25">
-        <v>4066</v>
+        <v>4070</v>
       </c>
       <c r="I25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J25">
-        <v>154.19999999999999</v>
+        <v>141.69999999999999</v>
       </c>
       <c r="K25">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>0.3</v>
@@ -2249,7 +2246,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>4118</v>
+        <v>4167</v>
       </c>
       <c r="B26" t="s">
         <v>96</v>
@@ -2258,7 +2255,7 @@
         <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -2270,13 +2267,13 @@
         <v>2</v>
       </c>
       <c r="H26">
-        <v>4070</v>
+        <v>4063</v>
       </c>
       <c r="I26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J26">
-        <v>141.69999999999999</v>
+        <v>152.80000000000001</v>
       </c>
       <c r="K26">
         <v>37</v>
@@ -2285,12 +2282,12 @@
         <v>0.3</v>
       </c>
       <c r="M26" s="3">
-        <v>43546</v>
+        <v>43549</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>4167</v>
+        <v>4146</v>
       </c>
       <c r="B27" t="s">
         <v>97</v>
@@ -2299,10 +2296,10 @@
         <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -2311,27 +2308,27 @@
         <v>2</v>
       </c>
       <c r="H27">
-        <v>4063</v>
+        <v>4061</v>
       </c>
       <c r="I27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J27">
-        <v>152.80000000000001</v>
+        <v>154.69999999999999</v>
       </c>
       <c r="K27">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L27">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M27" s="3">
-        <v>43549</v>
+        <v>43550</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>4146</v>
+        <v>4098</v>
       </c>
       <c r="B28" t="s">
         <v>98</v>
@@ -2340,45 +2337,45 @@
         <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="H28">
-        <v>4061</v>
+        <v>4067</v>
       </c>
       <c r="I28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J28">
-        <v>154.69999999999999</v>
+        <v>174.9</v>
       </c>
       <c r="K28">
-        <v>38</v>
+        <v>38.5</v>
       </c>
       <c r="L28">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M28" s="3">
-        <v>43550</v>
+        <v>43551</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>4098</v>
+        <v>3964</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -2390,115 +2387,115 @@
         <v>11</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>4067</v>
+        <v>3958</v>
       </c>
       <c r="I29" t="s">
-        <v>102</v>
-      </c>
-      <c r="J29">
-        <v>174.9</v>
-      </c>
-      <c r="K29">
-        <v>38.5</v>
-      </c>
-      <c r="L29">
-        <v>0.3</v>
-      </c>
-      <c r="M29" s="3">
-        <v>43551</v>
+        <v>100</v>
+      </c>
+      <c r="J29" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" t="s">
+        <v>106</v>
+      </c>
+      <c r="L29" t="s">
+        <v>106</v>
+      </c>
+      <c r="M29" s="1">
+        <v>42929</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>3964</v>
+        <v>3981</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>3958</v>
+        <v>3961</v>
       </c>
       <c r="I30" t="s">
-        <v>102</v>
-      </c>
-      <c r="J30" t="s">
-        <v>108</v>
-      </c>
-      <c r="K30" t="s">
-        <v>108</v>
+        <v>100</v>
+      </c>
+      <c r="J30">
+        <v>148</v>
+      </c>
+      <c r="K30">
+        <v>36</v>
       </c>
       <c r="L30" t="s">
-        <v>108</v>
-      </c>
-      <c r="M30" s="1">
-        <v>42929</v>
+        <v>106</v>
+      </c>
+      <c r="M30" s="3">
+        <v>42935</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>3981</v>
+        <v>4022</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E31" t="s">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>3961</v>
+        <v>3946</v>
       </c>
       <c r="I31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J31">
         <v>148</v>
       </c>
       <c r="K31">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M31" s="3">
-        <v>42935</v>
+        <v>42941</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>4022</v>
+        <v>3991</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -2510,42 +2507,42 @@
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <v>3946</v>
+        <v>3948</v>
       </c>
       <c r="I32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J32">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="K32">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="L32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M32" s="3">
-        <v>42941</v>
+        <v>42942</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3991</v>
+        <v>4016</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
@@ -2557,30 +2554,30 @@
         <v>1</v>
       </c>
       <c r="H33">
-        <v>3948</v>
+        <v>3947</v>
       </c>
       <c r="I33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J33">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="K33">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M33" s="3">
-        <v>42942</v>
+        <v>42943</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>4016</v>
+        <v>4029</v>
       </c>
       <c r="B34" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
@@ -2592,36 +2589,36 @@
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
-        <v>3947</v>
+        <v>3949</v>
       </c>
       <c r="I34" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J34">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="K34">
         <v>36</v>
       </c>
       <c r="L34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M34" s="3">
-        <v>42943</v>
+        <v>42944</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>4029</v>
+        <v>3992</v>
       </c>
       <c r="B35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
@@ -2630,39 +2627,39 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35">
-        <v>3949</v>
+        <v>3948</v>
       </c>
       <c r="I35" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J35">
-        <v>157</v>
+        <v>124</v>
       </c>
       <c r="K35">
         <v>36</v>
       </c>
       <c r="L35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M35" s="3">
-        <v>42944</v>
+        <v>42948</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>3992</v>
+        <v>4026</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
@@ -2671,48 +2668,48 @@
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
-        <v>3948</v>
+        <v>3946</v>
       </c>
       <c r="I36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J36">
-        <v>124</v>
+        <v>167</v>
       </c>
       <c r="K36">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L36" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M36" s="3">
-        <v>42948</v>
+        <v>42949</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>4026</v>
+        <v>3967</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F37" t="s">
         <v>11</v>
@@ -2721,71 +2718,71 @@
         <v>1</v>
       </c>
       <c r="H37">
-        <v>3946</v>
+        <v>3958</v>
       </c>
       <c r="I37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J37">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="K37">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L37" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M37" s="3">
-        <v>42949</v>
+        <v>42950</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>3967</v>
+        <v>4045</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E38" t="s">
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>3958</v>
+        <v>3954</v>
       </c>
       <c r="I38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J38">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="K38">
-        <v>35</v>
+        <v>38.5</v>
       </c>
       <c r="L38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M38" s="3">
-        <v>42950</v>
+        <v>42961</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>4045</v>
+        <v>4002</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
@@ -2797,45 +2794,45 @@
         <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39">
-        <v>3954</v>
+        <v>3955</v>
       </c>
       <c r="I39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J39">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="K39">
-        <v>38.5</v>
+        <v>34</v>
       </c>
       <c r="L39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M39" s="3">
-        <v>42961</v>
+        <v>42963</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>4002</v>
+        <v>4043</v>
       </c>
       <c r="B40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
         <v>11</v>
@@ -2844,80 +2841,80 @@
         <v>1</v>
       </c>
       <c r="H40">
-        <v>3955</v>
+        <v>3954</v>
       </c>
       <c r="I40" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J40">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="K40">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M40" s="3">
-        <v>42963</v>
+        <v>42964</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>4043</v>
+        <v>4000</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E41" t="s">
         <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G41">
         <v>1</v>
       </c>
       <c r="H41">
-        <v>3954</v>
+        <v>3955</v>
       </c>
       <c r="I41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J41">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="K41">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L41" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M41" s="3">
-        <v>42964</v>
+        <v>42970</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>4000</v>
+        <v>4010</v>
       </c>
       <c r="B42" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
@@ -2926,71 +2923,71 @@
         <v>1</v>
       </c>
       <c r="H42">
-        <v>3955</v>
+        <v>3957</v>
       </c>
       <c r="I42" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J42">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="K42">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M42" s="3">
-        <v>42970</v>
+        <v>42971</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>4010</v>
+        <v>4038</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>3957</v>
+        <v>3956</v>
       </c>
       <c r="I43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J43">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K43">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M43" s="3">
-        <v>42971</v>
+        <v>42972</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>4038</v>
+        <v>4036</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -2999,7 +2996,7 @@
         <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
         <v>11</v>
@@ -3011,27 +3008,27 @@
         <v>3956</v>
       </c>
       <c r="I44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J44">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K44">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M44" s="3">
-        <v>42972</v>
+        <v>42975</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>4036</v>
+        <v>4007</v>
       </c>
       <c r="B45" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
@@ -3043,45 +3040,45 @@
         <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45">
-        <v>3956</v>
+        <v>3957</v>
       </c>
       <c r="I45" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J45">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K45">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M45" s="3">
-        <v>42975</v>
+        <v>42977</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>4007</v>
+        <v>3982</v>
       </c>
       <c r="B46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F46" t="s">
         <v>14</v>
@@ -3090,71 +3087,71 @@
         <v>1</v>
       </c>
       <c r="H46">
-        <v>3957</v>
+        <v>3961</v>
       </c>
       <c r="I46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J46">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="K46">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M46" s="3">
-        <v>42977</v>
+        <v>42979</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>3982</v>
+        <v>4019</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47">
-        <v>3961</v>
+        <v>3947</v>
       </c>
       <c r="I47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J47">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="K47">
-        <v>35</v>
+        <v>33.5</v>
       </c>
       <c r="L47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M47" s="3">
-        <v>42979</v>
+        <v>42983</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>4019</v>
+        <v>4126</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
@@ -3163,45 +3160,45 @@
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F48" t="s">
         <v>11</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H48">
-        <v>3947</v>
+        <v>4065</v>
       </c>
       <c r="I48" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J48">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="K48">
-        <v>33.5</v>
-      </c>
-      <c r="L48" t="s">
-        <v>108</v>
+        <v>36</v>
+      </c>
+      <c r="L48">
+        <v>0.6</v>
       </c>
       <c r="M48" s="3">
-        <v>42983</v>
+        <v>43322</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>4126</v>
+        <v>4142</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E49" t="s">
         <v>10</v>
@@ -3213,19 +3210,19 @@
         <v>2</v>
       </c>
       <c r="H49">
-        <v>4065</v>
+        <v>4061</v>
       </c>
       <c r="I49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J49">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K49">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L49">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="M49" s="3">
         <v>43322</v>
@@ -3233,10 +3230,10 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>4142</v>
+        <v>4134</v>
       </c>
       <c r="B50" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -3248,36 +3245,36 @@
         <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G50">
         <v>2</v>
       </c>
       <c r="H50">
-        <v>4061</v>
+        <v>4076</v>
       </c>
       <c r="I50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J50">
-        <v>143</v>
+        <v>147.6</v>
       </c>
       <c r="K50">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L50">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="M50" s="3">
-        <v>43322</v>
+        <v>43325</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>4134</v>
+        <v>4154</v>
       </c>
       <c r="B51" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
@@ -3295,16 +3292,16 @@
         <v>2</v>
       </c>
       <c r="H51">
-        <v>4076</v>
+        <v>4062</v>
       </c>
       <c r="I51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J51">
-        <v>147.6</v>
+        <v>167.1</v>
       </c>
       <c r="K51">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L51">
         <v>0.6</v>
@@ -3315,51 +3312,51 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>4154</v>
+        <v>4081</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G52">
         <v>2</v>
       </c>
       <c r="H52">
-        <v>4062</v>
+        <v>4072</v>
       </c>
       <c r="I52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J52">
-        <v>167.1</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="K52">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L52">
         <v>0.6</v>
       </c>
       <c r="M52" s="3">
-        <v>43325</v>
+        <v>43327</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>4081</v>
+        <v>4097</v>
       </c>
       <c r="B53" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
@@ -3377,19 +3374,19 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>4072</v>
+        <v>4067</v>
       </c>
       <c r="I53" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J53">
-        <v>160.80000000000001</v>
+        <v>159.19999999999999</v>
       </c>
       <c r="K53">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L53">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="M53" s="3">
         <v>43327</v>
@@ -3397,16 +3394,16 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>4097</v>
+        <v>4089</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E54" t="s">
         <v>20</v>
@@ -3418,77 +3415,77 @@
         <v>2</v>
       </c>
       <c r="H54">
-        <v>4067</v>
+        <v>4064</v>
       </c>
       <c r="I54" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J54">
-        <v>159.19999999999999</v>
+        <v>166.2</v>
       </c>
       <c r="K54">
         <v>37</v>
       </c>
       <c r="L54">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="M54" s="3">
-        <v>43327</v>
+        <v>43328</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>4089</v>
+        <v>4143</v>
       </c>
       <c r="B55" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G55">
         <v>2</v>
       </c>
       <c r="H55">
-        <v>4064</v>
+        <v>4061</v>
       </c>
       <c r="I55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J55">
-        <v>166.2</v>
+        <v>159.1</v>
       </c>
       <c r="K55">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L55">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="M55" s="3">
-        <v>43328</v>
+        <v>43332</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>4143</v>
+        <v>4169</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E56" t="s">
         <v>20</v>
@@ -3500,19 +3497,19 @@
         <v>2</v>
       </c>
       <c r="H56">
-        <v>4061</v>
+        <v>4063</v>
       </c>
       <c r="I56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J56">
-        <v>159.1</v>
+        <v>162</v>
       </c>
       <c r="K56">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L56">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M56" s="3">
         <v>43332</v>
@@ -3520,16 +3517,16 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>4169</v>
+        <v>4106</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E57" t="s">
         <v>20</v>
@@ -3541,33 +3538,33 @@
         <v>2</v>
       </c>
       <c r="H57">
-        <v>4063</v>
+        <v>4066</v>
       </c>
       <c r="I57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J57">
-        <v>162</v>
+        <v>152.1</v>
       </c>
       <c r="K57">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L57">
         <v>0.2</v>
       </c>
       <c r="M57" s="3">
-        <v>43332</v>
+        <v>43333</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>4106</v>
+        <v>4013</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
@@ -3579,74 +3576,74 @@
         <v>14</v>
       </c>
       <c r="G58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H58">
-        <v>4066</v>
+        <v>3957</v>
       </c>
       <c r="I58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J58">
-        <v>152.1</v>
+        <v>125.4</v>
       </c>
       <c r="K58">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L58">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
       <c r="M58" s="3">
-        <v>43333</v>
+        <v>43122</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>4013</v>
+        <v>4056</v>
       </c>
       <c r="B59" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
         <v>43</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E59" t="s">
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="H59">
-        <v>3957</v>
+        <v>3945</v>
       </c>
       <c r="I59" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J59">
-        <v>125.4</v>
+        <v>157.5</v>
       </c>
       <c r="K59">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L59">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="M59" s="3">
-        <v>43122</v>
+        <v>43130</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>4056</v>
+        <v>4040</v>
       </c>
       <c r="B60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
         <v>43</v>
@@ -3658,124 +3655,124 @@
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60">
-        <v>3945</v>
+        <v>3956</v>
       </c>
       <c r="I60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J60">
-        <v>157.5</v>
+        <v>153.9</v>
       </c>
       <c r="K60">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L60">
         <v>2.4</v>
       </c>
       <c r="M60" s="3">
-        <v>43130</v>
+        <v>43129</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>4040</v>
+        <v>3986</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61">
-        <v>3956</v>
+        <v>3961</v>
       </c>
       <c r="I61" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J61">
-        <v>153.9</v>
+        <v>142</v>
       </c>
       <c r="K61">
-        <v>36.5</v>
+        <v>38</v>
       </c>
       <c r="L61">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="M61" s="3">
-        <v>43129</v>
+        <v>43131</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>3986</v>
+        <v>4028</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C62" t="s">
         <v>43</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
       </c>
       <c r="F62" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
       <c r="H62">
-        <v>3961</v>
+        <v>3946</v>
       </c>
       <c r="I62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J62">
-        <v>142</v>
+        <v>133.80000000000001</v>
       </c>
       <c r="K62">
         <v>38</v>
       </c>
       <c r="L62">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="M62" s="3">
-        <v>43131</v>
+        <v>43123</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>4028</v>
+        <v>4006</v>
       </c>
       <c r="B63" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C63" t="s">
         <v>43</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E63" t="s">
         <v>20</v>
@@ -3787,30 +3784,30 @@
         <v>1</v>
       </c>
       <c r="H63">
-        <v>3946</v>
+        <v>3955</v>
       </c>
       <c r="I63" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J63">
-        <v>133.80000000000001</v>
+        <v>134.9</v>
       </c>
       <c r="K63">
-        <v>38</v>
+        <v>37.5</v>
       </c>
       <c r="L63">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
       <c r="M63" s="3">
-        <v>43123</v>
+        <v>43119</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>4006</v>
+        <v>4042</v>
       </c>
       <c r="B64" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C64" t="s">
         <v>43</v>
@@ -3822,42 +3819,42 @@
         <v>20</v>
       </c>
       <c r="F64" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
       <c r="H64">
-        <v>3955</v>
+        <v>3956</v>
       </c>
       <c r="I64" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J64">
-        <v>134.9</v>
+        <v>137.30000000000001</v>
       </c>
       <c r="K64">
         <v>37.5</v>
       </c>
       <c r="L64">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="M64" s="3">
-        <v>43119</v>
+        <v>43132</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>4042</v>
+        <v>4035</v>
       </c>
       <c r="B65" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C65" t="s">
         <v>43</v>
       </c>
       <c r="D65" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E65" t="s">
         <v>20</v>
@@ -3869,71 +3866,71 @@
         <v>1</v>
       </c>
       <c r="H65">
-        <v>3956</v>
+        <v>3949</v>
       </c>
       <c r="I65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J65">
-        <v>137.30000000000001</v>
+        <v>150.30000000000001</v>
       </c>
       <c r="K65">
-        <v>37.5</v>
+        <v>38</v>
       </c>
       <c r="L65">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="M65" s="3">
-        <v>43132</v>
+        <v>43140</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>4035</v>
+        <v>4048</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C66" t="s">
         <v>43</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
       </c>
       <c r="F66" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
       <c r="H66">
-        <v>3949</v>
+        <v>3954</v>
       </c>
       <c r="I66" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J66">
-        <v>150.30000000000001</v>
+        <v>134.19999999999999</v>
       </c>
       <c r="K66">
         <v>38</v>
       </c>
       <c r="L66">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="M66" s="3">
-        <v>43140</v>
+        <v>43124</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>4048</v>
+        <v>3997</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C67" t="s">
         <v>43</v>
@@ -3942,45 +3939,45 @@
         <v>12</v>
       </c>
       <c r="E67" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F67" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G67">
         <v>1</v>
       </c>
       <c r="H67">
-        <v>3954</v>
+        <v>3948</v>
       </c>
       <c r="I67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J67">
-        <v>134.19999999999999</v>
+        <v>128.6</v>
       </c>
       <c r="K67">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L67">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="M67" s="3">
-        <v>43124</v>
+        <v>43146</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>3997</v>
+        <v>4011</v>
       </c>
       <c r="B68" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C68" t="s">
         <v>43</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E68" t="s">
         <v>10</v>
@@ -3992,30 +3989,30 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>3948</v>
+        <v>3957</v>
       </c>
       <c r="I68" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J68">
-        <v>128.6</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="K68">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L68">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="M68" s="3">
-        <v>43146</v>
+        <v>43138</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>4011</v>
+        <v>3970</v>
       </c>
       <c r="B69" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
         <v>43</v>
@@ -4033,36 +4030,36 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>3957</v>
+        <v>3958</v>
       </c>
       <c r="I69" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J69">
-        <v>141.80000000000001</v>
+        <v>185.8</v>
       </c>
       <c r="K69">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L69">
         <v>1.2</v>
       </c>
       <c r="M69" s="3">
-        <v>43138</v>
+        <v>43143</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3970</v>
+        <v>3976</v>
       </c>
       <c r="B70" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C70" t="s">
         <v>43</v>
       </c>
       <c r="D70" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E70" t="s">
         <v>10</v>
@@ -4074,30 +4071,30 @@
         <v>1</v>
       </c>
       <c r="H70">
-        <v>3958</v>
+        <v>3959</v>
       </c>
       <c r="I70" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J70">
-        <v>185.8</v>
+        <v>114</v>
       </c>
       <c r="K70">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L70">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="M70" s="3">
-        <v>43143</v>
+        <v>43110</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>3976</v>
+        <v>4054</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C71" t="s">
         <v>43</v>
@@ -4109,36 +4106,36 @@
         <v>10</v>
       </c>
       <c r="F71" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G71">
         <v>1</v>
       </c>
       <c r="H71">
-        <v>3959</v>
+        <v>3945</v>
       </c>
       <c r="I71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J71">
-        <v>114</v>
+        <v>116.5</v>
       </c>
       <c r="K71">
-        <v>36.5</v>
+        <v>37.5</v>
       </c>
       <c r="L71">
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="M71" s="3">
-        <v>43110</v>
+        <v>43125</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>4054</v>
+        <v>3989</v>
       </c>
       <c r="B72" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C72" t="s">
         <v>43</v>
@@ -4156,36 +4153,36 @@
         <v>1</v>
       </c>
       <c r="H72">
-        <v>3945</v>
+        <v>3961</v>
       </c>
       <c r="I72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J72">
-        <v>116.5</v>
+        <v>126.3</v>
       </c>
       <c r="K72">
-        <v>37.5</v>
+        <v>38</v>
       </c>
       <c r="L72">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="M72" s="3">
-        <v>43125</v>
+        <v>43126</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>3989</v>
+        <v>4050</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C73" t="s">
         <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -4197,36 +4194,36 @@
         <v>1</v>
       </c>
       <c r="H73">
-        <v>3961</v>
+        <v>3954</v>
       </c>
       <c r="I73" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J73">
-        <v>126.3</v>
+        <v>141.30000000000001</v>
       </c>
       <c r="K73">
         <v>38</v>
       </c>
       <c r="L73">
-        <v>3.9</v>
+        <v>1.5</v>
       </c>
       <c r="M73" s="3">
-        <v>43126</v>
+        <v>43133</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>4050</v>
+        <v>3975</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
         <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -4238,36 +4235,36 @@
         <v>1</v>
       </c>
       <c r="H74">
-        <v>3954</v>
+        <v>3959</v>
       </c>
       <c r="I74" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J74">
-        <v>141.30000000000001</v>
+        <v>116.6</v>
       </c>
       <c r="K74">
-        <v>38</v>
+        <v>35.5</v>
       </c>
       <c r="L74">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="M74" s="3">
-        <v>43133</v>
+        <v>43136</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>3975</v>
+        <v>4014</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C75" t="s">
         <v>43</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
@@ -4279,77 +4276,77 @@
         <v>1</v>
       </c>
       <c r="H75">
-        <v>3959</v>
+        <v>3957</v>
       </c>
       <c r="I75" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J75">
-        <v>116.6</v>
+        <v>138.1</v>
       </c>
       <c r="K75">
         <v>35.5</v>
       </c>
       <c r="L75">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="M75" s="3">
-        <v>43136</v>
+        <v>43137</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>4014</v>
+        <v>4017</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C76" t="s">
         <v>43</v>
       </c>
       <c r="D76" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
       </c>
       <c r="F76" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G76">
         <v>1</v>
       </c>
       <c r="H76">
-        <v>3957</v>
+        <v>3947</v>
       </c>
       <c r="I76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J76">
-        <v>138.1</v>
+        <v>133.6</v>
       </c>
       <c r="K76">
-        <v>35.5</v>
+        <v>37</v>
       </c>
       <c r="L76">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="M76" s="3">
-        <v>43137</v>
+        <v>43144</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>4017</v>
+        <v>4004</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C77" t="s">
         <v>43</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -4361,36 +4358,36 @@
         <v>1</v>
       </c>
       <c r="H77">
-        <v>3947</v>
+        <v>3955</v>
       </c>
       <c r="I77" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J77">
-        <v>133.6</v>
+        <v>134.6</v>
       </c>
       <c r="K77">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L77">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="M77" s="3">
-        <v>43144</v>
+        <v>43145</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>4004</v>
+        <v>4152</v>
       </c>
       <c r="B78" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C78" t="s">
         <v>43</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E78" t="s">
         <v>10</v>
@@ -4399,33 +4396,33 @@
         <v>11</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H78">
-        <v>3955</v>
+        <v>4063</v>
       </c>
       <c r="I78" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J78">
-        <v>134.6</v>
+        <v>101.5</v>
       </c>
       <c r="K78">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L78">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="M78" s="3">
-        <v>43145</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>4152</v>
+        <v>4161</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C79" t="s">
         <v>43</v>
@@ -4434,28 +4431,28 @@
         <v>12</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G79">
         <v>2</v>
       </c>
       <c r="H79">
-        <v>4063</v>
+        <v>4062</v>
       </c>
       <c r="I79" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J79">
-        <v>101.5</v>
+        <v>115.8</v>
       </c>
       <c r="K79">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="L79">
-        <v>5.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="M79" s="3">
         <v>43472</v>
@@ -4463,63 +4460,63 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>4161</v>
+        <v>4172</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C80" t="s">
         <v>43</v>
       </c>
       <c r="D80" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E80" t="s">
         <v>20</v>
       </c>
       <c r="F80" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G80">
         <v>2</v>
       </c>
       <c r="H80">
-        <v>4062</v>
+        <v>4064</v>
       </c>
       <c r="I80" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J80">
-        <v>115.8</v>
+        <v>157.19999999999999</v>
       </c>
       <c r="K80">
         <v>37</v>
       </c>
       <c r="L80">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M80" s="3">
-        <v>43472</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>4172</v>
+        <v>4173</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C81" t="s">
         <v>43</v>
       </c>
       <c r="D81" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F81" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G81">
         <v>2</v>
@@ -4528,16 +4525,16 @@
         <v>4064</v>
       </c>
       <c r="I81" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J81">
-        <v>157.19999999999999</v>
+        <v>110.3</v>
       </c>
       <c r="K81">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L81">
-        <v>2.2000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="M81" s="3">
         <v>43473</v>
@@ -4545,10 +4542,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>4173</v>
+        <v>4188</v>
       </c>
       <c r="B82" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C82" t="s">
         <v>43</v>
@@ -4566,30 +4563,30 @@
         <v>2</v>
       </c>
       <c r="H82">
-        <v>4064</v>
+        <v>4077</v>
       </c>
       <c r="I82" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J82">
-        <v>110.3</v>
+        <v>124.7</v>
       </c>
       <c r="K82">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L82">
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="M82" s="3">
-        <v>43473</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>4188</v>
+        <v>4117</v>
       </c>
       <c r="B83" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C83" t="s">
         <v>43</v>
@@ -4598,39 +4595,39 @@
         <v>12</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F83" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G83">
         <v>2</v>
       </c>
       <c r="H83">
-        <v>4077</v>
+        <v>4070</v>
       </c>
       <c r="I83" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J83">
-        <v>124.7</v>
+        <v>132.5</v>
       </c>
       <c r="K83">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L83">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="M83" s="3">
-        <v>43474</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>4117</v>
+        <v>4148</v>
       </c>
       <c r="B84" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C84" t="s">
         <v>43</v>
@@ -4648,109 +4645,68 @@
         <v>2</v>
       </c>
       <c r="H84">
-        <v>4070</v>
+        <v>4061</v>
       </c>
       <c r="I84" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J84">
-        <v>132.5</v>
+        <v>119.2</v>
       </c>
       <c r="K84">
-        <v>37</v>
+        <v>34.5</v>
       </c>
       <c r="L84">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="M84" s="3">
-        <v>43475</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>4148</v>
+        <v>4115</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C85" t="s">
         <v>43</v>
       </c>
       <c r="D85" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E85" t="s">
         <v>20</v>
       </c>
       <c r="F85" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G85">
         <v>2</v>
       </c>
       <c r="H85">
-        <v>4061</v>
+        <v>4066</v>
       </c>
       <c r="I85" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J85">
-        <v>119.2</v>
+        <v>121.6</v>
       </c>
       <c r="K85">
-        <v>34.5</v>
+        <v>34</v>
       </c>
       <c r="L85">
-        <v>3.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M85" s="3">
         <v>43479</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>4115</v>
-      </c>
-      <c r="B86" t="s">
-        <v>70</v>
-      </c>
-      <c r="C86" t="s">
-        <v>43</v>
-      </c>
-      <c r="D86" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" t="s">
-        <v>20</v>
-      </c>
-      <c r="F86" t="s">
-        <v>14</v>
-      </c>
-      <c r="G86">
-        <v>2</v>
-      </c>
-      <c r="H86">
-        <v>4066</v>
-      </c>
-      <c r="I86" t="s">
-        <v>102</v>
-      </c>
-      <c r="J86">
-        <v>121.6</v>
-      </c>
-      <c r="K86">
-        <v>34</v>
-      </c>
-      <c r="L86">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M86" s="3">
-        <v>43479</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L86">
-    <sortCondition ref="B1:B86"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L85">
+    <sortCondition ref="B1:B85"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Deleted phantom extra column
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B9461B1-3CE5-486A-B496-AC07F6C2E157}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BFFD020-2D3B-469E-BE3A-A3F6E9A9A0BA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -1205,20 +1205,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A4" sqref="A4:XFD4"/>
+      <selection pane="topRight" activeCell="N8" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="13" max="13" width="14" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1258,9 +1257,8 @@
       <c r="M1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3998</v>
       </c>
@@ -1301,7 +1299,7 @@
         <v>43167</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3987</v>
       </c>
@@ -1342,7 +1340,7 @@
         <v>43171</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4023</v>
       </c>
@@ -1383,7 +1381,7 @@
         <v>43175</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3993</v>
       </c>
@@ -1424,7 +1422,7 @@
         <v>43178</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4033</v>
       </c>
@@ -1465,7 +1463,7 @@
         <v>43179</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3985</v>
       </c>
@@ -1506,7 +1504,7 @@
         <v>43180</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3999</v>
       </c>
@@ -1547,7 +1545,7 @@
         <v>43181</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3990</v>
       </c>
@@ -1588,7 +1586,7 @@
         <v>43185</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4012</v>
       </c>
@@ -1629,7 +1627,7 @@
         <v>43186</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4025</v>
       </c>
@@ -1670,7 +1668,7 @@
         <v>43188</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4046</v>
       </c>
@@ -1711,7 +1709,7 @@
         <v>43189</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4119</v>
       </c>
@@ -1752,7 +1750,7 @@
         <v>43536</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4130</v>
       </c>
@@ -1793,7 +1791,7 @@
         <v>43536</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4128</v>
       </c>
@@ -1834,7 +1832,7 @@
         <v>43537</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4108</v>
       </c>
@@ -1875,7 +1873,7 @@
         <v>43537</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4150</v>
       </c>
@@ -1916,7 +1914,7 @@
         <v>43538</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4085</v>
       </c>
@@ -1957,7 +1955,7 @@
         <v>43539</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4127</v>
       </c>
@@ -1998,7 +1996,7 @@
         <v>43542</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4090</v>
       </c>
@@ -2039,7 +2037,7 @@
         <v>43543</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4116</v>
       </c>
@@ -2080,7 +2078,7 @@
         <v>43544</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4095</v>
       </c>
@@ -2121,7 +2119,7 @@
         <v>43545</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4155</v>
       </c>
@@ -2162,7 +2160,7 @@
         <v>43545</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4110</v>
       </c>
@@ -2203,7 +2201,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4118</v>
       </c>
@@ -2244,7 +2242,7 @@
         <v>43546</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4167</v>
       </c>
@@ -2285,7 +2283,7 @@
         <v>43549</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4146</v>
       </c>
@@ -2326,7 +2324,7 @@
         <v>43550</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>4098</v>
       </c>
@@ -2367,7 +2365,7 @@
         <v>43551</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3964</v>
       </c>
@@ -2408,7 +2406,7 @@
         <v>42929</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3981</v>
       </c>
@@ -2449,7 +2447,7 @@
         <v>42935</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4022</v>
       </c>
@@ -2490,7 +2488,7 @@
         <v>42941</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3991</v>
       </c>
@@ -2531,7 +2529,7 @@
         <v>42942</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4016</v>
       </c>
@@ -2572,7 +2570,7 @@
         <v>42943</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4029</v>
       </c>
@@ -2613,7 +2611,7 @@
         <v>42944</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3992</v>
       </c>
@@ -2654,7 +2652,7 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4026</v>
       </c>
@@ -2695,7 +2693,7 @@
         <v>42949</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>3967</v>
       </c>
@@ -2736,7 +2734,7 @@
         <v>42950</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4045</v>
       </c>
@@ -2777,7 +2775,7 @@
         <v>42961</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4002</v>
       </c>
@@ -2818,7 +2816,7 @@
         <v>42963</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4043</v>
       </c>
@@ -2859,7 +2857,7 @@
         <v>42964</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4000</v>
       </c>
@@ -2900,7 +2898,7 @@
         <v>42970</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>4010</v>
       </c>
@@ -2941,7 +2939,7 @@
         <v>42971</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4038</v>
       </c>
@@ -2982,7 +2980,7 @@
         <v>42972</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4036</v>
       </c>
@@ -3023,7 +3021,7 @@
         <v>42975</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4007</v>
       </c>
@@ -3064,7 +3062,7 @@
         <v>42977</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>3982</v>
       </c>
@@ -3105,7 +3103,7 @@
         <v>42979</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>4019</v>
       </c>
@@ -3146,7 +3144,7 @@
         <v>42983</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>4126</v>
       </c>
@@ -3187,7 +3185,7 @@
         <v>43322</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4142</v>
       </c>
@@ -3228,7 +3226,7 @@
         <v>43322</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>4134</v>
       </c>
@@ -3269,7 +3267,7 @@
         <v>43325</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>4154</v>
       </c>
@@ -3310,7 +3308,7 @@
         <v>43325</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>4081</v>
       </c>
@@ -3351,7 +3349,7 @@
         <v>43327</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4097</v>
       </c>
@@ -3392,7 +3390,7 @@
         <v>43327</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>4089</v>
       </c>
@@ -3433,7 +3431,7 @@
         <v>43328</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>4143</v>
       </c>
@@ -3474,7 +3472,7 @@
         <v>43332</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>4169</v>
       </c>
@@ -3515,7 +3513,7 @@
         <v>43332</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>4106</v>
       </c>
@@ -3556,7 +3554,7 @@
         <v>43333</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>4013</v>
       </c>
@@ -3597,7 +3595,7 @@
         <v>43122</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>4056</v>
       </c>
@@ -3638,7 +3636,7 @@
         <v>43130</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>4040</v>
       </c>
@@ -3679,7 +3677,7 @@
         <v>43129</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>3986</v>
       </c>
@@ -3720,7 +3718,7 @@
         <v>43131</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4028</v>
       </c>
@@ -3761,7 +3759,7 @@
         <v>43123</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4006</v>
       </c>
@@ -3802,7 +3800,7 @@
         <v>43119</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>4042</v>
       </c>
@@ -3843,7 +3841,7 @@
         <v>43132</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4035</v>
       </c>
@@ -3884,7 +3882,7 @@
         <v>43140</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>4048</v>
       </c>
@@ -3925,7 +3923,7 @@
         <v>43124</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3997</v>
       </c>
@@ -3966,7 +3964,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4011</v>
       </c>
@@ -4007,7 +4005,7 @@
         <v>43138</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>3970</v>
       </c>
@@ -4048,7 +4046,7 @@
         <v>43143</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>3976</v>
       </c>
@@ -4089,7 +4087,7 @@
         <v>43110</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>4054</v>
       </c>
@@ -4130,7 +4128,7 @@
         <v>43125</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>3989</v>
       </c>
@@ -4171,7 +4169,7 @@
         <v>43126</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4050</v>
       </c>
@@ -4212,7 +4210,7 @@
         <v>43133</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>3975</v>
       </c>
@@ -4253,7 +4251,7 @@
         <v>43136</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>4014</v>
       </c>
@@ -4294,7 +4292,7 @@
         <v>43137</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>4017</v>
       </c>
@@ -4335,7 +4333,7 @@
         <v>43144</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4004</v>
       </c>
@@ -4376,7 +4374,7 @@
         <v>43145</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>4152</v>
       </c>
@@ -4417,7 +4415,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4161</v>
       </c>
@@ -4458,7 +4456,7 @@
         <v>43472</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>4172</v>
       </c>
@@ -4499,7 +4497,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4173</v>
       </c>
@@ -4540,7 +4538,7 @@
         <v>43473</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>4188</v>
       </c>
@@ -4581,7 +4579,7 @@
         <v>43474</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4117</v>
       </c>
@@ -4622,7 +4620,7 @@
         <v>43475</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>4148</v>
       </c>
@@ -4663,7 +4661,7 @@
         <v>43479</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>4115</v>
       </c>

</xml_diff>

<commit_message>
Deleted S11 (urea squirrel)
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BFFD020-2D3B-469E-BE3A-A3F6E9A9A0BA}"/>
+  <xr:revisionPtr revIDLastSave="279" documentId="8_{6754E49E-8D3C-4C0C-A782-6D445CEBCE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5FBA919-0D56-47FB-91CF-8382B170C283}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="912" windowWidth="12960" windowHeight="12048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="108">
   <si>
     <t>Number</t>
   </si>
@@ -352,9 +352,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>S11</t>
   </si>
   <si>
     <t>Date_Sampled</t>
@@ -1205,11 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N8" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,7 +1251,7 @@
         <v>105</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2654,19 +2650,19 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>4026</v>
+        <v>3967</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F36" t="s">
         <v>11</v>
@@ -2675,71 +2671,71 @@
         <v>1</v>
       </c>
       <c r="H36">
-        <v>3946</v>
+        <v>3958</v>
       </c>
       <c r="I36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J36">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="K36">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L36" t="s">
         <v>106</v>
       </c>
       <c r="M36" s="3">
-        <v>42949</v>
+        <v>42950</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>3967</v>
+        <v>4045</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>3958</v>
+        <v>3954</v>
       </c>
       <c r="I37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J37">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="K37">
-        <v>35</v>
+        <v>38.5</v>
       </c>
       <c r="L37" t="s">
         <v>106</v>
       </c>
       <c r="M37" s="3">
-        <v>42950</v>
+        <v>42961</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>4045</v>
+        <v>4002</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
@@ -2751,45 +2747,45 @@
         <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
-        <v>3954</v>
+        <v>3955</v>
       </c>
       <c r="I38" t="s">
         <v>101</v>
       </c>
       <c r="J38">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="K38">
-        <v>38.5</v>
+        <v>34</v>
       </c>
       <c r="L38" t="s">
         <v>106</v>
       </c>
       <c r="M38" s="3">
-        <v>42961</v>
+        <v>42963</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>4002</v>
+        <v>4043</v>
       </c>
       <c r="B39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
         <v>11</v>
@@ -2798,80 +2794,80 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>3955</v>
+        <v>3954</v>
       </c>
       <c r="I39" t="s">
         <v>101</v>
       </c>
       <c r="J39">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="K39">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L39" t="s">
         <v>106</v>
       </c>
       <c r="M39" s="3">
-        <v>42963</v>
+        <v>42964</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>4043</v>
+        <v>4000</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E40" t="s">
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>3954</v>
+        <v>3955</v>
       </c>
       <c r="I40" t="s">
         <v>101</v>
       </c>
       <c r="J40">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="K40">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L40" t="s">
         <v>106</v>
       </c>
       <c r="M40" s="3">
-        <v>42964</v>
+        <v>42970</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>4000</v>
+        <v>4010</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -2880,71 +2876,71 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>3955</v>
+        <v>3957</v>
       </c>
       <c r="I41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J41">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="K41">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L41" t="s">
         <v>106</v>
       </c>
       <c r="M41" s="3">
-        <v>42970</v>
+        <v>42971</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>4010</v>
+        <v>4038</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42">
-        <v>3957</v>
+        <v>3956</v>
       </c>
       <c r="I42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J42">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="K42">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L42" t="s">
         <v>106</v>
       </c>
       <c r="M42" s="3">
-        <v>42971</v>
+        <v>42972</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>4038</v>
+        <v>4036</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -2953,7 +2949,7 @@
         <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
@@ -2968,24 +2964,24 @@
         <v>101</v>
       </c>
       <c r="J43">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K43">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L43" t="s">
         <v>106</v>
       </c>
       <c r="M43" s="3">
-        <v>42972</v>
+        <v>42975</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>4036</v>
+        <v>4007</v>
       </c>
       <c r="B44" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
@@ -2997,45 +2993,45 @@
         <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>3956</v>
+        <v>3957</v>
       </c>
       <c r="I44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J44">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K44">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="L44" t="s">
         <v>106</v>
       </c>
       <c r="M44" s="3">
-        <v>42975</v>
+        <v>42977</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>4007</v>
+        <v>3982</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -3044,71 +3040,71 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>3957</v>
+        <v>3961</v>
       </c>
       <c r="I45" t="s">
         <v>100</v>
       </c>
       <c r="J45">
-        <v>213</v>
+        <v>158</v>
       </c>
       <c r="K45">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L45" t="s">
         <v>106</v>
       </c>
       <c r="M45" s="3">
-        <v>42977</v>
+        <v>42979</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>3982</v>
+        <v>4019</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
       <c r="H46">
-        <v>3961</v>
+        <v>3947</v>
       </c>
       <c r="I46" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J46">
-        <v>158</v>
+        <v>211</v>
       </c>
       <c r="K46">
-        <v>35</v>
+        <v>33.5</v>
       </c>
       <c r="L46" t="s">
         <v>106</v>
       </c>
       <c r="M46" s="3">
-        <v>42979</v>
+        <v>42983</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>4019</v>
+        <v>4126</v>
       </c>
       <c r="B47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
@@ -3117,45 +3113,45 @@
         <v>12</v>
       </c>
       <c r="E47" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F47" t="s">
         <v>11</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47">
-        <v>3947</v>
+        <v>4065</v>
       </c>
       <c r="I47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J47">
-        <v>211</v>
+        <v>162</v>
       </c>
       <c r="K47">
-        <v>33.5</v>
-      </c>
-      <c r="L47" t="s">
-        <v>106</v>
+        <v>36</v>
+      </c>
+      <c r="L47">
+        <v>0.6</v>
       </c>
       <c r="M47" s="3">
-        <v>42983</v>
+        <v>43322</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>4126</v>
+        <v>4142</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E48" t="s">
         <v>10</v>
@@ -3167,19 +3163,19 @@
         <v>2</v>
       </c>
       <c r="H48">
-        <v>4065</v>
+        <v>4061</v>
       </c>
       <c r="I48" t="s">
         <v>100</v>
       </c>
       <c r="J48">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="K48">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L48">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="M48" s="3">
         <v>43322</v>
@@ -3187,10 +3183,10 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>4142</v>
+        <v>4134</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -3202,36 +3198,36 @@
         <v>10</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G49">
         <v>2</v>
       </c>
       <c r="H49">
-        <v>4061</v>
+        <v>4076</v>
       </c>
       <c r="I49" t="s">
         <v>100</v>
       </c>
       <c r="J49">
-        <v>143</v>
+        <v>147.6</v>
       </c>
       <c r="K49">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L49">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="M49" s="3">
-        <v>43322</v>
+        <v>43325</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>4134</v>
+        <v>4154</v>
       </c>
       <c r="B50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
@@ -3249,16 +3245,16 @@
         <v>2</v>
       </c>
       <c r="H50">
-        <v>4076</v>
+        <v>4062</v>
       </c>
       <c r="I50" t="s">
         <v>100</v>
       </c>
       <c r="J50">
-        <v>147.6</v>
+        <v>167.1</v>
       </c>
       <c r="K50">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L50">
         <v>0.6</v>
@@ -3269,51 +3265,51 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>4154</v>
+        <v>4081</v>
       </c>
       <c r="B51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F51" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
       <c r="H51">
-        <v>4062</v>
+        <v>4072</v>
       </c>
       <c r="I51" t="s">
         <v>100</v>
       </c>
       <c r="J51">
-        <v>167.1</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="K51">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L51">
         <v>0.6</v>
       </c>
       <c r="M51" s="3">
-        <v>43325</v>
+        <v>43327</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>4081</v>
+        <v>4097</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
@@ -3331,19 +3327,19 @@
         <v>2</v>
       </c>
       <c r="H52">
-        <v>4072</v>
+        <v>4067</v>
       </c>
       <c r="I52" t="s">
         <v>100</v>
       </c>
       <c r="J52">
-        <v>160.80000000000001</v>
+        <v>159.19999999999999</v>
       </c>
       <c r="K52">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L52">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="M52" s="3">
         <v>43327</v>
@@ -3351,16 +3347,16 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>4097</v>
+        <v>4089</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
@@ -3372,77 +3368,77 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>4067</v>
+        <v>4064</v>
       </c>
       <c r="I53" t="s">
         <v>100</v>
       </c>
       <c r="J53">
-        <v>159.19999999999999</v>
+        <v>166.2</v>
       </c>
       <c r="K53">
         <v>37</v>
       </c>
       <c r="L53">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="M53" s="3">
-        <v>43327</v>
+        <v>43328</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>4089</v>
+        <v>4143</v>
       </c>
       <c r="B54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E54" t="s">
         <v>20</v>
       </c>
       <c r="F54" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G54">
         <v>2</v>
       </c>
       <c r="H54">
-        <v>4064</v>
+        <v>4061</v>
       </c>
       <c r="I54" t="s">
         <v>100</v>
       </c>
       <c r="J54">
-        <v>166.2</v>
+        <v>159.1</v>
       </c>
       <c r="K54">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L54">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="M54" s="3">
-        <v>43328</v>
+        <v>43332</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>4143</v>
+        <v>4169</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
@@ -3454,19 +3450,19 @@
         <v>2</v>
       </c>
       <c r="H55">
-        <v>4061</v>
+        <v>4063</v>
       </c>
       <c r="I55" t="s">
         <v>100</v>
       </c>
       <c r="J55">
-        <v>159.1</v>
+        <v>162</v>
       </c>
       <c r="K55">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L55">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M55" s="3">
         <v>43332</v>
@@ -3474,16 +3470,16 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>4169</v>
+        <v>4106</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E56" t="s">
         <v>20</v>
@@ -3495,33 +3491,33 @@
         <v>2</v>
       </c>
       <c r="H56">
-        <v>4063</v>
+        <v>4066</v>
       </c>
       <c r="I56" t="s">
         <v>100</v>
       </c>
       <c r="J56">
-        <v>162</v>
+        <v>152.1</v>
       </c>
       <c r="K56">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L56">
         <v>0.2</v>
       </c>
       <c r="M56" s="3">
-        <v>43332</v>
+        <v>43333</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>4106</v>
+        <v>4013</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -3533,74 +3529,74 @@
         <v>14</v>
       </c>
       <c r="G57">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H57">
-        <v>4066</v>
+        <v>3957</v>
       </c>
       <c r="I57" t="s">
         <v>100</v>
       </c>
       <c r="J57">
-        <v>152.1</v>
+        <v>125.4</v>
       </c>
       <c r="K57">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L57">
-        <v>0.2</v>
+        <v>1.6</v>
       </c>
       <c r="M57" s="3">
-        <v>43333</v>
+        <v>43122</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>4013</v>
+        <v>4056</v>
       </c>
       <c r="B58" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C58" t="s">
         <v>43</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E58" t="s">
         <v>20</v>
       </c>
       <c r="F58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
       <c r="H58">
-        <v>3957</v>
+        <v>3945</v>
       </c>
       <c r="I58" t="s">
         <v>100</v>
       </c>
       <c r="J58">
-        <v>125.4</v>
+        <v>157.5</v>
       </c>
       <c r="K58">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L58">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="M58" s="3">
-        <v>43122</v>
+        <v>43130</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>4056</v>
+        <v>4040</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C59" t="s">
         <v>43</v>
@@ -3612,124 +3608,124 @@
         <v>20</v>
       </c>
       <c r="F59" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
       <c r="H59">
-        <v>3945</v>
+        <v>3956</v>
       </c>
       <c r="I59" t="s">
         <v>100</v>
       </c>
       <c r="J59">
-        <v>157.5</v>
+        <v>153.9</v>
       </c>
       <c r="K59">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L59">
         <v>2.4</v>
       </c>
       <c r="M59" s="3">
-        <v>43130</v>
+        <v>43129</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>4040</v>
+        <v>3986</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
         <v>43</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E60" t="s">
         <v>20</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
       <c r="H60">
-        <v>3956</v>
+        <v>3961</v>
       </c>
       <c r="I60" t="s">
         <v>100</v>
       </c>
       <c r="J60">
-        <v>153.9</v>
+        <v>142</v>
       </c>
       <c r="K60">
-        <v>36.5</v>
+        <v>38</v>
       </c>
       <c r="L60">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="M60" s="3">
-        <v>43129</v>
+        <v>43131</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>3986</v>
+        <v>4028</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
         <v>20</v>
       </c>
       <c r="F61" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
       <c r="H61">
-        <v>3961</v>
+        <v>3946</v>
       </c>
       <c r="I61" t="s">
         <v>100</v>
       </c>
       <c r="J61">
-        <v>142</v>
+        <v>133.80000000000001</v>
       </c>
       <c r="K61">
         <v>38</v>
       </c>
       <c r="L61">
-        <v>2.1</v>
+        <v>2.8</v>
       </c>
       <c r="M61" s="3">
-        <v>43131</v>
+        <v>43123</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>4028</v>
+        <v>4006</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C62" t="s">
         <v>43</v>
       </c>
       <c r="D62" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E62" t="s">
         <v>20</v>
@@ -3741,30 +3737,30 @@
         <v>1</v>
       </c>
       <c r="H62">
-        <v>3946</v>
+        <v>3955</v>
       </c>
       <c r="I62" t="s">
         <v>100</v>
       </c>
       <c r="J62">
-        <v>133.80000000000001</v>
+        <v>134.9</v>
       </c>
       <c r="K62">
-        <v>38</v>
+        <v>37.5</v>
       </c>
       <c r="L62">
-        <v>2.8</v>
+        <v>1.7</v>
       </c>
       <c r="M62" s="3">
-        <v>43123</v>
+        <v>43119</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>4006</v>
+        <v>4042</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C63" t="s">
         <v>43</v>
@@ -3776,42 +3772,42 @@
         <v>20</v>
       </c>
       <c r="F63" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
       <c r="H63">
-        <v>3955</v>
+        <v>3956</v>
       </c>
       <c r="I63" t="s">
         <v>100</v>
       </c>
       <c r="J63">
-        <v>134.9</v>
+        <v>137.30000000000001</v>
       </c>
       <c r="K63">
         <v>37.5</v>
       </c>
       <c r="L63">
-        <v>1.7</v>
+        <v>2.8</v>
       </c>
       <c r="M63" s="3">
-        <v>43119</v>
+        <v>43132</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>4042</v>
+        <v>4035</v>
       </c>
       <c r="B64" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
         <v>43</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
         <v>20</v>
@@ -3823,71 +3819,71 @@
         <v>1</v>
       </c>
       <c r="H64">
-        <v>3956</v>
+        <v>3949</v>
       </c>
       <c r="I64" t="s">
         <v>100</v>
       </c>
       <c r="J64">
-        <v>137.30000000000001</v>
+        <v>150.30000000000001</v>
       </c>
       <c r="K64">
-        <v>37.5</v>
+        <v>38</v>
       </c>
       <c r="L64">
-        <v>2.8</v>
+        <v>1.3</v>
       </c>
       <c r="M64" s="3">
-        <v>43132</v>
+        <v>43140</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>4035</v>
+        <v>4048</v>
       </c>
       <c r="B65" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C65" t="s">
         <v>43</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
         <v>20</v>
       </c>
       <c r="F65" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G65">
         <v>1</v>
       </c>
       <c r="H65">
-        <v>3949</v>
+        <v>3954</v>
       </c>
       <c r="I65" t="s">
         <v>100</v>
       </c>
       <c r="J65">
-        <v>150.30000000000001</v>
+        <v>134.19999999999999</v>
       </c>
       <c r="K65">
         <v>38</v>
       </c>
       <c r="L65">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="M65" s="3">
-        <v>43140</v>
+        <v>43124</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>4048</v>
+        <v>3997</v>
       </c>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C66" t="s">
         <v>43</v>
@@ -3896,45 +3892,45 @@
         <v>12</v>
       </c>
       <c r="E66" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F66" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
       <c r="H66">
-        <v>3954</v>
+        <v>3948</v>
       </c>
       <c r="I66" t="s">
         <v>100</v>
       </c>
       <c r="J66">
-        <v>134.19999999999999</v>
+        <v>128.6</v>
       </c>
       <c r="K66">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L66">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="M66" s="3">
-        <v>43124</v>
+        <v>43146</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>3997</v>
+        <v>4011</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C67" t="s">
         <v>43</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E67" t="s">
         <v>10</v>
@@ -3946,30 +3942,30 @@
         <v>1</v>
       </c>
       <c r="H67">
-        <v>3948</v>
+        <v>3957</v>
       </c>
       <c r="I67" t="s">
         <v>100</v>
       </c>
       <c r="J67">
-        <v>128.6</v>
+        <v>141.80000000000001</v>
       </c>
       <c r="K67">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L67">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="M67" s="3">
-        <v>43146</v>
+        <v>43138</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>4011</v>
+        <v>3970</v>
       </c>
       <c r="B68" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
         <v>43</v>
@@ -3987,36 +3983,36 @@
         <v>1</v>
       </c>
       <c r="H68">
-        <v>3957</v>
+        <v>3958</v>
       </c>
       <c r="I68" t="s">
         <v>100</v>
       </c>
       <c r="J68">
-        <v>141.80000000000001</v>
+        <v>185.8</v>
       </c>
       <c r="K68">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L68">
         <v>1.2</v>
       </c>
       <c r="M68" s="3">
-        <v>43138</v>
+        <v>43143</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>3970</v>
+        <v>3976</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C69" t="s">
         <v>43</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E69" t="s">
         <v>10</v>
@@ -4028,30 +4024,30 @@
         <v>1</v>
       </c>
       <c r="H69">
-        <v>3958</v>
+        <v>3959</v>
       </c>
       <c r="I69" t="s">
         <v>100</v>
       </c>
       <c r="J69">
-        <v>185.8</v>
+        <v>114</v>
       </c>
       <c r="K69">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L69">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="M69" s="3">
-        <v>43143</v>
+        <v>43110</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>3976</v>
+        <v>4054</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C70" t="s">
         <v>43</v>
@@ -4063,36 +4059,36 @@
         <v>10</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G70">
         <v>1</v>
       </c>
       <c r="H70">
-        <v>3959</v>
+        <v>3945</v>
       </c>
       <c r="I70" t="s">
         <v>100</v>
       </c>
       <c r="J70">
-        <v>114</v>
+        <v>116.5</v>
       </c>
       <c r="K70">
-        <v>36.5</v>
+        <v>37.5</v>
       </c>
       <c r="L70">
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="M70" s="3">
-        <v>43110</v>
+        <v>43125</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>4054</v>
+        <v>3989</v>
       </c>
       <c r="B71" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C71" t="s">
         <v>43</v>
@@ -4110,36 +4106,36 @@
         <v>1</v>
       </c>
       <c r="H71">
-        <v>3945</v>
+        <v>3961</v>
       </c>
       <c r="I71" t="s">
         <v>100</v>
       </c>
       <c r="J71">
-        <v>116.5</v>
+        <v>126.3</v>
       </c>
       <c r="K71">
-        <v>37.5</v>
+        <v>38</v>
       </c>
       <c r="L71">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="M71" s="3">
-        <v>43125</v>
+        <v>43126</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>3989</v>
+        <v>4050</v>
       </c>
       <c r="B72" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C72" t="s">
         <v>43</v>
       </c>
       <c r="D72" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E72" t="s">
         <v>10</v>
@@ -4151,36 +4147,36 @@
         <v>1</v>
       </c>
       <c r="H72">
-        <v>3961</v>
+        <v>3954</v>
       </c>
       <c r="I72" t="s">
         <v>100</v>
       </c>
       <c r="J72">
-        <v>126.3</v>
+        <v>141.30000000000001</v>
       </c>
       <c r="K72">
         <v>38</v>
       </c>
       <c r="L72">
-        <v>3.9</v>
+        <v>1.5</v>
       </c>
       <c r="M72" s="3">
-        <v>43126</v>
+        <v>43133</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>4050</v>
+        <v>3975</v>
       </c>
       <c r="B73" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
         <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
         <v>10</v>
@@ -4192,36 +4188,36 @@
         <v>1</v>
       </c>
       <c r="H73">
-        <v>3954</v>
+        <v>3959</v>
       </c>
       <c r="I73" t="s">
         <v>100</v>
       </c>
       <c r="J73">
-        <v>141.30000000000001</v>
+        <v>116.6</v>
       </c>
       <c r="K73">
-        <v>38</v>
+        <v>35.5</v>
       </c>
       <c r="L73">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="M73" s="3">
-        <v>43133</v>
+        <v>43136</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>3975</v>
+        <v>4014</v>
       </c>
       <c r="B74" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C74" t="s">
         <v>43</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E74" t="s">
         <v>10</v>
@@ -4233,77 +4229,77 @@
         <v>1</v>
       </c>
       <c r="H74">
-        <v>3959</v>
+        <v>3957</v>
       </c>
       <c r="I74" t="s">
         <v>100</v>
       </c>
       <c r="J74">
-        <v>116.6</v>
+        <v>138.1</v>
       </c>
       <c r="K74">
         <v>35.5</v>
       </c>
       <c r="L74">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="M74" s="3">
-        <v>43136</v>
+        <v>43137</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>4014</v>
+        <v>4017</v>
       </c>
       <c r="B75" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C75" t="s">
         <v>43</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E75" t="s">
         <v>10</v>
       </c>
       <c r="F75" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G75">
         <v>1</v>
       </c>
       <c r="H75">
-        <v>3957</v>
+        <v>3947</v>
       </c>
       <c r="I75" t="s">
         <v>100</v>
       </c>
       <c r="J75">
-        <v>138.1</v>
+        <v>133.6</v>
       </c>
       <c r="K75">
-        <v>35.5</v>
+        <v>37</v>
       </c>
       <c r="L75">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="M75" s="3">
-        <v>43137</v>
+        <v>43144</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>4017</v>
+        <v>4004</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C76" t="s">
         <v>43</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E76" t="s">
         <v>10</v>
@@ -4315,36 +4311,36 @@
         <v>1</v>
       </c>
       <c r="H76">
-        <v>3947</v>
+        <v>3955</v>
       </c>
       <c r="I76" t="s">
         <v>100</v>
       </c>
       <c r="J76">
-        <v>133.6</v>
+        <v>134.6</v>
       </c>
       <c r="K76">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L76">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="M76" s="3">
-        <v>43144</v>
+        <v>43145</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>4004</v>
+        <v>4152</v>
       </c>
       <c r="B77" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C77" t="s">
         <v>43</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E77" t="s">
         <v>10</v>
@@ -4353,33 +4349,33 @@
         <v>11</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H77">
-        <v>3955</v>
+        <v>4063</v>
       </c>
       <c r="I77" t="s">
         <v>100</v>
       </c>
       <c r="J77">
-        <v>134.6</v>
+        <v>101.5</v>
       </c>
       <c r="K77">
-        <v>36</v>
+        <v>36.5</v>
       </c>
       <c r="L77">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
       <c r="M77" s="3">
-        <v>43145</v>
+        <v>43472</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>4152</v>
+        <v>4161</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C78" t="s">
         <v>43</v>
@@ -4388,28 +4384,28 @@
         <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F78" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G78">
         <v>2</v>
       </c>
       <c r="H78">
-        <v>4063</v>
+        <v>4062</v>
       </c>
       <c r="I78" t="s">
         <v>100</v>
       </c>
       <c r="J78">
-        <v>101.5</v>
+        <v>115.8</v>
       </c>
       <c r="K78">
-        <v>36.5</v>
+        <v>37</v>
       </c>
       <c r="L78">
-        <v>5.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="M78" s="3">
         <v>43472</v>
@@ -4417,63 +4413,63 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>4161</v>
+        <v>4172</v>
       </c>
       <c r="B79" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C79" t="s">
         <v>43</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E79" t="s">
         <v>20</v>
       </c>
       <c r="F79" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G79">
         <v>2</v>
       </c>
       <c r="H79">
-        <v>4062</v>
+        <v>4064</v>
       </c>
       <c r="I79" t="s">
         <v>100</v>
       </c>
       <c r="J79">
-        <v>115.8</v>
+        <v>157.19999999999999</v>
       </c>
       <c r="K79">
         <v>37</v>
       </c>
       <c r="L79">
-        <v>2.2999999999999998</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M79" s="3">
-        <v>43472</v>
+        <v>43473</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>4172</v>
+        <v>4173</v>
       </c>
       <c r="B80" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C80" t="s">
         <v>43</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F80" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G80">
         <v>2</v>
@@ -4485,13 +4481,13 @@
         <v>100</v>
       </c>
       <c r="J80">
-        <v>157.19999999999999</v>
+        <v>110.3</v>
       </c>
       <c r="K80">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="L80">
-        <v>2.2000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="M80" s="3">
         <v>43473</v>
@@ -4499,10 +4495,10 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>4173</v>
+        <v>4188</v>
       </c>
       <c r="B81" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
         <v>43</v>
@@ -4520,30 +4516,30 @@
         <v>2</v>
       </c>
       <c r="H81">
-        <v>4064</v>
+        <v>4077</v>
       </c>
       <c r="I81" t="s">
         <v>100</v>
       </c>
       <c r="J81">
-        <v>110.3</v>
+        <v>124.7</v>
       </c>
       <c r="K81">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="L81">
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="M81" s="3">
-        <v>43473</v>
+        <v>43474</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>4188</v>
+        <v>4117</v>
       </c>
       <c r="B82" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C82" t="s">
         <v>43</v>
@@ -4552,39 +4548,39 @@
         <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F82" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G82">
         <v>2</v>
       </c>
       <c r="H82">
-        <v>4077</v>
+        <v>4070</v>
       </c>
       <c r="I82" t="s">
         <v>100</v>
       </c>
       <c r="J82">
-        <v>124.7</v>
+        <v>132.5</v>
       </c>
       <c r="K82">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L82">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="M82" s="3">
-        <v>43474</v>
+        <v>43475</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>4117</v>
+        <v>4148</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C83" t="s">
         <v>43</v>
@@ -4602,109 +4598,68 @@
         <v>2</v>
       </c>
       <c r="H83">
-        <v>4070</v>
+        <v>4061</v>
       </c>
       <c r="I83" t="s">
         <v>100</v>
       </c>
       <c r="J83">
-        <v>132.5</v>
+        <v>119.2</v>
       </c>
       <c r="K83">
-        <v>37</v>
+        <v>34.5</v>
       </c>
       <c r="L83">
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="M83" s="3">
-        <v>43475</v>
+        <v>43479</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>4148</v>
+        <v>4115</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C84" t="s">
         <v>43</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E84" t="s">
         <v>20</v>
       </c>
       <c r="F84" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G84">
         <v>2</v>
       </c>
       <c r="H84">
-        <v>4061</v>
+        <v>4066</v>
       </c>
       <c r="I84" t="s">
         <v>100</v>
       </c>
       <c r="J84">
-        <v>119.2</v>
+        <v>121.6</v>
       </c>
       <c r="K84">
-        <v>34.5</v>
+        <v>34</v>
       </c>
       <c r="L84">
-        <v>3.3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M84" s="3">
         <v>43479</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A85">
-        <v>4115</v>
-      </c>
-      <c r="B85" t="s">
-        <v>70</v>
-      </c>
-      <c r="C85" t="s">
-        <v>43</v>
-      </c>
-      <c r="D85" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" t="s">
-        <v>20</v>
-      </c>
-      <c r="F85" t="s">
-        <v>14</v>
-      </c>
-      <c r="G85">
-        <v>2</v>
-      </c>
-      <c r="H85">
-        <v>4066</v>
-      </c>
-      <c r="I85" t="s">
-        <v>100</v>
-      </c>
-      <c r="J85">
-        <v>121.6</v>
-      </c>
-      <c r="K85">
-        <v>34</v>
-      </c>
-      <c r="L85">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="M85" s="3">
-        <v>43479</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L85">
-    <sortCondition ref="B1:B85"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L84">
+    <sortCondition ref="B1:B84"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>